<commit_message>
Fix issues with summary repeat
</commit_message>
<xml_diff>
--- a/default/forms/app/delivery_plus_plus.xlsx
+++ b/default/forms/app/delivery_plus_plus.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="424">
   <si>
     <t>type</t>
   </si>
@@ -874,6 +874,66 @@
     <t xml:space="preserve">indexed-repeat(${birth_weight}, ${baby_repeat}, position(..))</t>
   </si>
   <si>
+    <t>current_danger_signs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indexed-repeat(${r_baby_danger_sign_present}, ${baby_repeat}, position(..))</t>
+  </si>
+  <si>
+    <t>current_infected_umbilical_cord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indexed-repeat(${infected_umbilical_cord}, ${baby_repeat}, position(..))</t>
+  </si>
+  <si>
+    <t>current_convulsion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indexed-repeat(${b_convulsion}, ${baby_repeat}, position(..))</t>
+  </si>
+  <si>
+    <t>current_difficulty_feeding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indexed-repeat(${difficulty_feeding}, ${baby_repeat}, position(..))</t>
+  </si>
+  <si>
+    <t>current_vomit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indexed-repeat(${vomit}, ${baby_repeat}, position(..))</t>
+  </si>
+  <si>
+    <t>current_drowsy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indexed-repeat(${drowsy}, ${baby_repeat}, position(..))</t>
+  </si>
+  <si>
+    <t>current_stiff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indexed-repeat(${stiff}, ${baby_repeat}, position(..))</t>
+  </si>
+  <si>
+    <t>current_yellow_skin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indexed-repeat(${yellow_skin}, ${baby_repeat}, position(..))</t>
+  </si>
+  <si>
+    <t>current_fever</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indexed-repeat(${b_fever}, ${baby_repeat}, position(..))</t>
+  </si>
+  <si>
+    <t>current_blue_skin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indexed-repeat(${blue_skin}, ${baby_repeat}, position(..))</t>
+  </si>
+  <si>
     <t>r_baby_header</t>
   </si>
   <si>
@@ -895,7 +955,7 @@
     <t xml:space="preserve">Weight: *${current_weight}*</t>
   </si>
   <si>
-    <t xml:space="preserve">indexed-repeat(${r_baby_danger_sign_present}, ${baby_repeat}, position(..)) = 'yes'</t>
+    <t xml:space="preserve">${current_danger_signs} = 'yes'</t>
   </si>
   <si>
     <t xml:space="preserve">h3 blue</t>
@@ -904,55 +964,55 @@
     <t>r_infected_umbilical_cord</t>
   </si>
   <si>
-    <t xml:space="preserve">indexed-repeat(${infected_umbilical_cord}, ${baby_repeat}, position(..)) = 'yes'</t>
+    <t xml:space="preserve">${current_infected_umbilical_cord} = 'yes'</t>
   </si>
   <si>
     <t>r_convulsion</t>
   </si>
   <si>
-    <t xml:space="preserve">indexed-repeat(${b_convulsion}, ${baby_repeat}, position(..)) = 'yes'</t>
+    <t xml:space="preserve">${current_convulsion} = 'yes'</t>
   </si>
   <si>
     <t>r_difficulty_feeding</t>
   </si>
   <si>
-    <t xml:space="preserve">indexed-repeat(${difficulty_feeding}, ${baby_repeat}, position(..)) = 'yes'</t>
+    <t xml:space="preserve">${current_difficulty_feeding} = 'yes'</t>
   </si>
   <si>
     <t>r_vomit</t>
   </si>
   <si>
-    <t xml:space="preserve">indexed-repeat(${vomit}, ${baby_repeat}, position(..)) = 'yes'</t>
+    <t xml:space="preserve">${current_vomit} = 'yes'</t>
   </si>
   <si>
     <t>r_drowsy</t>
   </si>
   <si>
-    <t xml:space="preserve">indexed-repeat(${drowsy}, ${baby_repeat}, position(..)) = 'yes'</t>
+    <t xml:space="preserve">${current_drowsy} = 'yes'</t>
   </si>
   <si>
     <t>r_stiff</t>
   </si>
   <si>
-    <t xml:space="preserve">indexed-repeat(${stiff}, ${baby_repeat}, position(..)) = 'yes'</t>
+    <t xml:space="preserve">${current_stiff} = 'yes'</t>
   </si>
   <si>
     <t>r_yellow_skin</t>
   </si>
   <si>
-    <t xml:space="preserve">indexed-repeat(${yellow_skin}, ${baby_repeat}, position(..)) = 'yes'</t>
+    <t xml:space="preserve">${current_yellow_skin} = 'yes'</t>
   </si>
   <si>
     <t>r_fever</t>
   </si>
   <si>
-    <t xml:space="preserve">indexed-repeat(${b_fever}, ${baby_repeat}, position(..)) = 'yes'</t>
+    <t xml:space="preserve">${current_fever} = 'yes'</t>
   </si>
   <si>
     <t>r_blue_skin</t>
   </si>
   <si>
-    <t xml:space="preserve">indexed-repeat(${blue_skin}, ${baby_repeat}, position(..)) = 'yes'</t>
+    <t xml:space="preserve">${current_blue_skin} = 'yes'</t>
   </si>
   <si>
     <t>r_referrals</t>
@@ -1426,8 +1486,6 @@
     <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="3" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
       <protection hidden="0" locked="1"/>
@@ -1437,6 +1495,8 @@
     <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -1898,8 +1958,8 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="1" showRowColHeaders="1" showZeros="1" topLeftCell="A67" zoomScale="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView showGridLines="1" showRowColHeaders="1" showZeros="1" zoomScale="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -4037,21 +4097,21 @@
       <c r="AMJ75" s="11"/>
     </row>
     <row r="76" s="11" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A76" s="16" t="s">
+      <c r="A76" s="13" t="s">
         <v>167</v>
       </c>
       <c r="B76" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="C76" s="17" t="s">
+      <c r="C76" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="D76" s="17" t="s">
+      <c r="D76" s="11" t="s">
         <v>52</v>
       </c>
       <c r="E76" s="11"/>
       <c r="F76" s="15"/>
-      <c r="G76" s="18" t="s">
+      <c r="G76" s="16" t="s">
         <v>170</v>
       </c>
       <c r="H76" s="11"/>
@@ -4486,1787 +4546,2038 @@
       <c r="AMJ93" s="11"/>
     </row>
     <row r="94" ht="12.75"/>
-    <row r="95" s="19" customFormat="1" ht="12.75">
-      <c r="A95" s="20" t="s">
+    <row r="95" s="17" customFormat="1" ht="12.75">
+      <c r="A95" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B95" s="20" t="s">
+      <c r="B95" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="C95" s="19" t="s">
+      <c r="C95" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D95" s="19"/>
-      <c r="E95" s="19"/>
-      <c r="F95" s="19"/>
-      <c r="G95" s="19" t="s">
+      <c r="D95" s="17"/>
+      <c r="E95" s="17"/>
+      <c r="F95" s="17"/>
+      <c r="G95" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="H95" s="19"/>
-      <c r="I95" s="19"/>
-      <c r="J95" s="19"/>
-      <c r="K95" s="19"/>
-      <c r="L95" s="19"/>
-      <c r="M95" s="19"/>
-      <c r="N95" s="19"/>
-      <c r="AMF95" s="19"/>
-      <c r="AMG95" s="19"/>
-      <c r="AMH95" s="19"/>
-      <c r="AMI95" s="19"/>
-      <c r="AMJ95" s="19"/>
-    </row>
-    <row r="96" s="19" customFormat="1" ht="12.75">
-      <c r="A96" s="20" t="s">
+      <c r="H95" s="17"/>
+      <c r="I95" s="17"/>
+      <c r="J95" s="17"/>
+      <c r="K95" s="17"/>
+      <c r="L95" s="17"/>
+      <c r="M95" s="17"/>
+      <c r="N95" s="17"/>
+      <c r="AMF95" s="17"/>
+      <c r="AMG95" s="17"/>
+      <c r="AMH95" s="17"/>
+      <c r="AMI95" s="17"/>
+      <c r="AMJ95" s="17"/>
+    </row>
+    <row r="96" s="17" customFormat="1" ht="12.75">
+      <c r="A96" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B96" s="20" t="s">
+      <c r="B96" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="C96" s="19" t="s">
+      <c r="C96" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="D96" s="19"/>
-      <c r="E96" s="19"/>
-      <c r="F96" s="19"/>
-      <c r="G96" s="19"/>
-      <c r="H96" s="19"/>
-      <c r="I96" s="19"/>
-      <c r="J96" s="19"/>
-      <c r="K96" s="19"/>
-      <c r="L96" s="19"/>
-      <c r="M96" s="19"/>
-      <c r="N96" s="19"/>
-      <c r="AMF96" s="19"/>
-      <c r="AMG96" s="19"/>
-      <c r="AMH96" s="19"/>
-      <c r="AMI96" s="19"/>
-      <c r="AMJ96" s="19"/>
-    </row>
-    <row r="97" s="19" customFormat="1" ht="12.75">
-      <c r="A97" s="20" t="s">
+      <c r="D96" s="17"/>
+      <c r="E96" s="17"/>
+      <c r="F96" s="17"/>
+      <c r="G96" s="17"/>
+      <c r="H96" s="17"/>
+      <c r="I96" s="17"/>
+      <c r="J96" s="17"/>
+      <c r="K96" s="17"/>
+      <c r="L96" s="17"/>
+      <c r="M96" s="17"/>
+      <c r="N96" s="17"/>
+      <c r="AMF96" s="17"/>
+      <c r="AMG96" s="17"/>
+      <c r="AMH96" s="17"/>
+      <c r="AMI96" s="17"/>
+      <c r="AMJ96" s="17"/>
+    </row>
+    <row r="97" s="17" customFormat="1" ht="12.75">
+      <c r="A97" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B97" s="20" t="s">
+      <c r="B97" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="C97" s="19" t="s">
+      <c r="C97" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="D97" s="19"/>
-      <c r="E97" s="19"/>
-      <c r="F97" s="19"/>
-      <c r="G97" s="19" t="s">
+      <c r="D97" s="17"/>
+      <c r="E97" s="17"/>
+      <c r="F97" s="17"/>
+      <c r="G97" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="H97" s="19"/>
-      <c r="I97" s="19"/>
-      <c r="J97" s="19"/>
-      <c r="K97" s="19"/>
-      <c r="L97" s="19"/>
-      <c r="M97" s="19"/>
-      <c r="N97" s="19"/>
-      <c r="AMF97" s="19"/>
-      <c r="AMG97" s="19"/>
-      <c r="AMH97" s="19"/>
-      <c r="AMI97" s="19"/>
-      <c r="AMJ97" s="19"/>
-    </row>
-    <row r="98" s="19" customFormat="1" ht="12.75">
-      <c r="A98" s="20" t="s">
+      <c r="H97" s="17"/>
+      <c r="I97" s="17"/>
+      <c r="J97" s="17"/>
+      <c r="K97" s="17"/>
+      <c r="L97" s="17"/>
+      <c r="M97" s="17"/>
+      <c r="N97" s="17"/>
+      <c r="AMF97" s="17"/>
+      <c r="AMG97" s="17"/>
+      <c r="AMH97" s="17"/>
+      <c r="AMI97" s="17"/>
+      <c r="AMJ97" s="17"/>
+    </row>
+    <row r="98" s="17" customFormat="1" ht="12.75">
+      <c r="A98" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B98" s="20" t="s">
+      <c r="B98" s="18" t="s">
         <v>209</v>
       </c>
-      <c r="C98" s="19" t="s">
+      <c r="C98" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="D98" s="19"/>
-      <c r="E98" s="19"/>
-      <c r="F98" s="19"/>
-      <c r="G98" s="19"/>
-      <c r="H98" s="19"/>
-      <c r="I98" s="19"/>
-      <c r="J98" s="19"/>
-      <c r="K98" s="19"/>
-      <c r="L98" s="19"/>
-      <c r="M98" s="19"/>
-      <c r="N98" s="19"/>
-      <c r="AMF98" s="19"/>
-      <c r="AMG98" s="19"/>
-      <c r="AMH98" s="19"/>
-      <c r="AMI98" s="19"/>
-      <c r="AMJ98" s="19"/>
-    </row>
-    <row r="99" s="19" customFormat="1" ht="12.75">
-      <c r="A99" s="20" t="s">
+      <c r="D98" s="17"/>
+      <c r="E98" s="17"/>
+      <c r="F98" s="17"/>
+      <c r="G98" s="17"/>
+      <c r="H98" s="17"/>
+      <c r="I98" s="17"/>
+      <c r="J98" s="17"/>
+      <c r="K98" s="17"/>
+      <c r="L98" s="17"/>
+      <c r="M98" s="17"/>
+      <c r="N98" s="17"/>
+      <c r="AMF98" s="17"/>
+      <c r="AMG98" s="17"/>
+      <c r="AMH98" s="17"/>
+      <c r="AMI98" s="17"/>
+      <c r="AMJ98" s="17"/>
+    </row>
+    <row r="99" s="17" customFormat="1" ht="12.75">
+      <c r="A99" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B99" s="20" t="s">
+      <c r="B99" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="C99" s="19" t="s">
+      <c r="C99" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="D99" s="19"/>
-      <c r="E99" s="19"/>
-      <c r="F99" s="19"/>
-      <c r="G99" s="19" t="s">
+      <c r="D99" s="17"/>
+      <c r="E99" s="17"/>
+      <c r="F99" s="17"/>
+      <c r="G99" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="H99" s="19"/>
-      <c r="I99" s="19"/>
-      <c r="J99" s="19"/>
-      <c r="K99" s="19"/>
-      <c r="L99" s="19"/>
-      <c r="M99" s="19"/>
-      <c r="N99" s="19"/>
-      <c r="AMF99" s="19"/>
-      <c r="AMG99" s="19"/>
-      <c r="AMH99" s="19"/>
-      <c r="AMI99" s="19"/>
-      <c r="AMJ99" s="19"/>
-    </row>
-    <row r="100" s="19" customFormat="1" ht="12.75">
-      <c r="A100" s="20" t="s">
+      <c r="H99" s="17"/>
+      <c r="I99" s="17"/>
+      <c r="J99" s="17"/>
+      <c r="K99" s="17"/>
+      <c r="L99" s="17"/>
+      <c r="M99" s="17"/>
+      <c r="N99" s="17"/>
+      <c r="AMF99" s="17"/>
+      <c r="AMG99" s="17"/>
+      <c r="AMH99" s="17"/>
+      <c r="AMI99" s="17"/>
+      <c r="AMJ99" s="17"/>
+    </row>
+    <row r="100" s="17" customFormat="1" ht="12.75">
+      <c r="A100" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B100" s="20" t="s">
+      <c r="B100" s="18" t="s">
         <v>213</v>
       </c>
-      <c r="C100" s="19" t="s">
+      <c r="C100" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="D100" s="19"/>
-      <c r="E100" s="19"/>
-      <c r="F100" s="19"/>
-      <c r="G100" s="19" t="s">
+      <c r="D100" s="17"/>
+      <c r="E100" s="17"/>
+      <c r="F100" s="17"/>
+      <c r="G100" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="H100" s="19"/>
-      <c r="I100" s="19"/>
-      <c r="J100" s="19"/>
-      <c r="K100" s="19"/>
-      <c r="L100" s="19"/>
-      <c r="M100" s="19"/>
-      <c r="AMF100" s="19"/>
-      <c r="AMG100" s="19"/>
-      <c r="AMH100" s="19"/>
-      <c r="AMI100" s="19"/>
-      <c r="AMJ100" s="19"/>
-    </row>
-    <row r="101" s="19" customFormat="1" ht="12.75">
-      <c r="A101" s="20" t="s">
+      <c r="H100" s="17"/>
+      <c r="I100" s="17"/>
+      <c r="J100" s="17"/>
+      <c r="K100" s="17"/>
+      <c r="L100" s="17"/>
+      <c r="M100" s="17"/>
+      <c r="AMF100" s="17"/>
+      <c r="AMG100" s="17"/>
+      <c r="AMH100" s="17"/>
+      <c r="AMI100" s="17"/>
+      <c r="AMJ100" s="17"/>
+    </row>
+    <row r="101" s="17" customFormat="1" ht="12.75">
+      <c r="A101" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B101" s="20" t="s">
+      <c r="B101" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="C101" s="19" t="s">
+      <c r="C101" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="D101" s="19"/>
-      <c r="E101" s="19" t="s">
+      <c r="D101" s="17"/>
+      <c r="E101" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="F101" s="19"/>
-      <c r="G101" s="19" t="s">
+      <c r="F101" s="17"/>
+      <c r="G101" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H101" s="19"/>
-      <c r="I101" s="19"/>
-      <c r="J101" s="19"/>
-      <c r="K101" s="19"/>
-      <c r="L101" s="19"/>
-      <c r="M101" s="19"/>
-      <c r="AMF101" s="19"/>
-      <c r="AMG101" s="19"/>
-      <c r="AMH101" s="19"/>
-      <c r="AMI101" s="19"/>
-      <c r="AMJ101" s="19"/>
-    </row>
-    <row r="102" s="19" customFormat="1" ht="12.75">
-      <c r="A102" s="20" t="s">
+      <c r="H101" s="17"/>
+      <c r="I101" s="17"/>
+      <c r="J101" s="17"/>
+      <c r="K101" s="17"/>
+      <c r="L101" s="17"/>
+      <c r="M101" s="17"/>
+      <c r="AMF101" s="17"/>
+      <c r="AMG101" s="17"/>
+      <c r="AMH101" s="17"/>
+      <c r="AMI101" s="17"/>
+      <c r="AMJ101" s="17"/>
+    </row>
+    <row r="102" s="17" customFormat="1" ht="12.75">
+      <c r="A102" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B102" s="20" t="s">
+      <c r="B102" s="18" t="s">
         <v>220</v>
       </c>
-      <c r="C102" s="19" t="s">
+      <c r="C102" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="D102" s="19"/>
-      <c r="E102" s="19" t="s">
+      <c r="D102" s="17"/>
+      <c r="E102" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="F102" s="19"/>
-      <c r="G102" s="19" t="s">
+      <c r="F102" s="17"/>
+      <c r="G102" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H102" s="19"/>
-      <c r="I102" s="19"/>
-      <c r="J102" s="19"/>
-      <c r="K102" s="19"/>
-      <c r="L102" s="19"/>
-      <c r="M102" s="19"/>
-      <c r="AMF102" s="19"/>
-      <c r="AMG102" s="19"/>
-      <c r="AMH102" s="19"/>
-      <c r="AMI102" s="19"/>
-      <c r="AMJ102" s="19"/>
-    </row>
-    <row r="103" s="19" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A103" s="20" t="s">
+      <c r="H102" s="17"/>
+      <c r="I102" s="17"/>
+      <c r="J102" s="17"/>
+      <c r="K102" s="17"/>
+      <c r="L102" s="17"/>
+      <c r="M102" s="17"/>
+      <c r="AMF102" s="17"/>
+      <c r="AMG102" s="17"/>
+      <c r="AMH102" s="17"/>
+      <c r="AMI102" s="17"/>
+      <c r="AMJ102" s="17"/>
+    </row>
+    <row r="103" s="17" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A103" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B103" s="20" t="s">
+      <c r="B103" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="C103" s="19" t="s">
+      <c r="C103" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="D103" s="19"/>
-      <c r="E103" s="21" t="s">
+      <c r="D103" s="17"/>
+      <c r="E103" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="F103" s="19"/>
-      <c r="G103" s="19" t="s">
+      <c r="F103" s="17"/>
+      <c r="G103" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="H103" s="19"/>
-      <c r="I103" s="19"/>
-      <c r="J103" s="19"/>
-      <c r="K103" s="19"/>
-      <c r="L103" s="19"/>
-      <c r="M103" s="19"/>
-      <c r="AMF103" s="19"/>
-      <c r="AMG103" s="19"/>
-      <c r="AMH103" s="19"/>
-      <c r="AMI103" s="19"/>
-      <c r="AMJ103" s="19"/>
-    </row>
-    <row r="104" s="19" customFormat="1" ht="12.75">
-      <c r="A104" s="20" t="s">
+      <c r="H103" s="17"/>
+      <c r="I103" s="17"/>
+      <c r="J103" s="17"/>
+      <c r="K103" s="17"/>
+      <c r="L103" s="17"/>
+      <c r="M103" s="17"/>
+      <c r="AMF103" s="17"/>
+      <c r="AMG103" s="17"/>
+      <c r="AMH103" s="17"/>
+      <c r="AMI103" s="17"/>
+      <c r="AMJ103" s="17"/>
+    </row>
+    <row r="104" s="17" customFormat="1" ht="12.75">
+      <c r="A104" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B104" s="20" t="s">
+      <c r="B104" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="C104" s="19" t="s">
+      <c r="C104" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="D104" s="19"/>
-      <c r="E104" s="19" t="s">
+      <c r="D104" s="17"/>
+      <c r="E104" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="F104" s="19"/>
-      <c r="G104" s="19" t="s">
+      <c r="F104" s="17"/>
+      <c r="G104" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H104" s="19"/>
-      <c r="I104" s="19"/>
-      <c r="J104" s="19"/>
-      <c r="K104" s="19"/>
-      <c r="L104" s="19"/>
-      <c r="M104" s="19"/>
-      <c r="AMF104" s="19"/>
-      <c r="AMG104" s="19"/>
-      <c r="AMH104" s="19"/>
-      <c r="AMI104" s="19"/>
-      <c r="AMJ104" s="19"/>
-    </row>
-    <row r="105" s="19" customFormat="1" ht="12.75">
-      <c r="A105" s="20" t="s">
+      <c r="H104" s="17"/>
+      <c r="I104" s="17"/>
+      <c r="J104" s="17"/>
+      <c r="K104" s="17"/>
+      <c r="L104" s="17"/>
+      <c r="M104" s="17"/>
+      <c r="AMF104" s="17"/>
+      <c r="AMG104" s="17"/>
+      <c r="AMH104" s="17"/>
+      <c r="AMI104" s="17"/>
+      <c r="AMJ104" s="17"/>
+    </row>
+    <row r="105" s="17" customFormat="1" ht="12.75">
+      <c r="A105" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B105" s="20" t="s">
+      <c r="B105" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="C105" s="19" t="s">
+      <c r="C105" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="D105" s="19"/>
-      <c r="E105" s="19" t="s">
+      <c r="D105" s="17"/>
+      <c r="E105" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="F105" s="19"/>
-      <c r="G105" s="19" t="s">
+      <c r="F105" s="17"/>
+      <c r="G105" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H105" s="19"/>
-      <c r="I105" s="19"/>
-      <c r="J105" s="19"/>
-      <c r="K105" s="19"/>
-      <c r="L105" s="19"/>
-      <c r="M105" s="19"/>
-      <c r="AMF105" s="19"/>
-      <c r="AMG105" s="19"/>
-      <c r="AMH105" s="19"/>
-      <c r="AMI105" s="19"/>
-      <c r="AMJ105" s="19"/>
-    </row>
-    <row r="106" s="19" customFormat="1" ht="12.75">
-      <c r="A106" s="20" t="s">
+      <c r="H105" s="17"/>
+      <c r="I105" s="17"/>
+      <c r="J105" s="17"/>
+      <c r="K105" s="17"/>
+      <c r="L105" s="17"/>
+      <c r="M105" s="17"/>
+      <c r="AMF105" s="17"/>
+      <c r="AMG105" s="17"/>
+      <c r="AMH105" s="17"/>
+      <c r="AMI105" s="17"/>
+      <c r="AMJ105" s="17"/>
+    </row>
+    <row r="106" s="17" customFormat="1" ht="12.75">
+      <c r="A106" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B106" s="20" t="s">
+      <c r="B106" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="C106" s="19" t="s">
+      <c r="C106" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="D106" s="19"/>
-      <c r="E106" s="19" t="s">
+      <c r="D106" s="17"/>
+      <c r="E106" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="F106" s="19"/>
-      <c r="G106" s="19" t="s">
+      <c r="F106" s="17"/>
+      <c r="G106" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H106" s="19"/>
-      <c r="I106" s="19"/>
-      <c r="J106" s="19"/>
-      <c r="K106" s="19"/>
-      <c r="L106" s="19"/>
-      <c r="M106" s="19"/>
-      <c r="AMF106" s="19"/>
-      <c r="AMG106" s="19"/>
-      <c r="AMH106" s="19"/>
-      <c r="AMI106" s="19"/>
-      <c r="AMJ106" s="19"/>
-    </row>
-    <row r="107" s="19" customFormat="1" ht="12.75">
-      <c r="A107" s="20" t="s">
+      <c r="H106" s="17"/>
+      <c r="I106" s="17"/>
+      <c r="J106" s="17"/>
+      <c r="K106" s="17"/>
+      <c r="L106" s="17"/>
+      <c r="M106" s="17"/>
+      <c r="AMF106" s="17"/>
+      <c r="AMG106" s="17"/>
+      <c r="AMH106" s="17"/>
+      <c r="AMI106" s="17"/>
+      <c r="AMJ106" s="17"/>
+    </row>
+    <row r="107" s="17" customFormat="1" ht="12.75">
+      <c r="A107" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B107" s="20" t="s">
+      <c r="B107" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="C107" s="19" t="s">
+      <c r="C107" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="D107" s="19"/>
-      <c r="E107" s="19" t="s">
+      <c r="D107" s="17"/>
+      <c r="E107" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="F107" s="19"/>
-      <c r="G107" s="19" t="s">
+      <c r="F107" s="17"/>
+      <c r="G107" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="H107" s="19"/>
-      <c r="I107" s="19"/>
-      <c r="J107" s="19"/>
-      <c r="K107" s="19"/>
-      <c r="L107" s="19"/>
-      <c r="M107" s="19"/>
-      <c r="AMF107" s="19"/>
-      <c r="AMG107" s="19"/>
-      <c r="AMH107" s="19"/>
-      <c r="AMI107" s="19"/>
-      <c r="AMJ107" s="19"/>
-    </row>
-    <row r="108" s="19" customFormat="1" ht="12.75">
-      <c r="A108" s="20" t="s">
+      <c r="H107" s="17"/>
+      <c r="I107" s="17"/>
+      <c r="J107" s="17"/>
+      <c r="K107" s="17"/>
+      <c r="L107" s="17"/>
+      <c r="M107" s="17"/>
+      <c r="AMF107" s="17"/>
+      <c r="AMG107" s="17"/>
+      <c r="AMH107" s="17"/>
+      <c r="AMI107" s="17"/>
+      <c r="AMJ107" s="17"/>
+    </row>
+    <row r="108" s="17" customFormat="1" ht="12.75">
+      <c r="A108" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B108" s="20" t="s">
+      <c r="B108" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="C108" s="19" t="s">
+      <c r="C108" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D108" s="19"/>
-      <c r="E108" s="19" t="s">
+      <c r="D108" s="17"/>
+      <c r="E108" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="F108" s="19"/>
-      <c r="G108" s="19" t="s">
+      <c r="F108" s="17"/>
+      <c r="G108" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H108" s="19"/>
-      <c r="I108" s="19"/>
-      <c r="J108" s="19"/>
-      <c r="K108" s="19"/>
-      <c r="L108" s="19"/>
-      <c r="M108" s="19"/>
-      <c r="AMF108" s="19"/>
-      <c r="AMG108" s="19"/>
-      <c r="AMH108" s="19"/>
-      <c r="AMI108" s="19"/>
-      <c r="AMJ108" s="19"/>
-    </row>
-    <row r="109" s="19" customFormat="1" ht="12.75">
-      <c r="A109" s="20" t="s">
+      <c r="H108" s="17"/>
+      <c r="I108" s="17"/>
+      <c r="J108" s="17"/>
+      <c r="K108" s="17"/>
+      <c r="L108" s="17"/>
+      <c r="M108" s="17"/>
+      <c r="AMF108" s="17"/>
+      <c r="AMG108" s="17"/>
+      <c r="AMH108" s="17"/>
+      <c r="AMI108" s="17"/>
+      <c r="AMJ108" s="17"/>
+    </row>
+    <row r="109" s="17" customFormat="1" ht="12.75">
+      <c r="A109" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B109" s="20" t="s">
+      <c r="B109" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="C109" s="19" t="s">
+      <c r="C109" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D109" s="19"/>
-      <c r="E109" s="19" t="s">
+      <c r="D109" s="17"/>
+      <c r="E109" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="F109" s="19"/>
-      <c r="G109" s="19" t="s">
+      <c r="F109" s="17"/>
+      <c r="G109" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H109" s="19"/>
-      <c r="I109" s="19"/>
-      <c r="J109" s="19"/>
-      <c r="K109" s="19"/>
-      <c r="L109" s="19"/>
-      <c r="M109" s="19"/>
-      <c r="O109" s="19"/>
-      <c r="AMF109" s="19"/>
-      <c r="AMG109" s="19"/>
-      <c r="AMH109" s="19"/>
-      <c r="AMI109" s="19"/>
-      <c r="AMJ109" s="19"/>
-    </row>
-    <row r="110" s="19" customFormat="1" ht="12.75">
-      <c r="A110" s="20" t="s">
+      <c r="H109" s="17"/>
+      <c r="I109" s="17"/>
+      <c r="J109" s="17"/>
+      <c r="K109" s="17"/>
+      <c r="L109" s="17"/>
+      <c r="M109" s="17"/>
+      <c r="O109" s="17"/>
+      <c r="AMF109" s="17"/>
+      <c r="AMG109" s="17"/>
+      <c r="AMH109" s="17"/>
+      <c r="AMI109" s="17"/>
+      <c r="AMJ109" s="17"/>
+    </row>
+    <row r="110" s="17" customFormat="1" ht="12.75">
+      <c r="A110" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B110" s="20" t="s">
+      <c r="B110" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="C110" s="19" t="s">
+      <c r="C110" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D110" s="19"/>
-      <c r="E110" s="19" t="s">
+      <c r="D110" s="17"/>
+      <c r="E110" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="F110" s="19"/>
-      <c r="G110" s="19" t="s">
+      <c r="F110" s="17"/>
+      <c r="G110" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H110" s="19"/>
-      <c r="I110" s="19"/>
-      <c r="J110" s="19"/>
-      <c r="K110" s="19"/>
-      <c r="L110" s="19"/>
-      <c r="M110" s="19"/>
-      <c r="O110" s="19"/>
-      <c r="AMF110" s="19"/>
-      <c r="AMG110" s="19"/>
-      <c r="AMH110" s="19"/>
-      <c r="AMI110" s="19"/>
-      <c r="AMJ110" s="19"/>
-    </row>
-    <row r="111" s="19" customFormat="1" ht="12.75">
-      <c r="A111" s="20" t="s">
+      <c r="H110" s="17"/>
+      <c r="I110" s="17"/>
+      <c r="J110" s="17"/>
+      <c r="K110" s="17"/>
+      <c r="L110" s="17"/>
+      <c r="M110" s="17"/>
+      <c r="O110" s="17"/>
+      <c r="AMF110" s="17"/>
+      <c r="AMG110" s="17"/>
+      <c r="AMH110" s="17"/>
+      <c r="AMI110" s="17"/>
+      <c r="AMJ110" s="17"/>
+    </row>
+    <row r="111" s="17" customFormat="1" ht="12.75">
+      <c r="A111" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B111" s="20" t="s">
+      <c r="B111" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="C111" s="19" t="s">
+      <c r="C111" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="D111" s="19"/>
-      <c r="E111" s="19" t="s">
+      <c r="D111" s="17"/>
+      <c r="E111" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="F111" s="19"/>
-      <c r="G111" s="19" t="s">
+      <c r="F111" s="17"/>
+      <c r="G111" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H111" s="19"/>
-      <c r="I111" s="19"/>
-      <c r="J111" s="19"/>
-      <c r="K111" s="19"/>
-      <c r="L111" s="19"/>
-      <c r="M111" s="19"/>
-      <c r="O111" s="19"/>
-      <c r="AMF111" s="19"/>
-      <c r="AMG111" s="19"/>
-      <c r="AMH111" s="19"/>
-      <c r="AMI111" s="19"/>
-      <c r="AMJ111" s="19"/>
-    </row>
-    <row r="112" s="19" customFormat="1" ht="12.75">
-      <c r="A112" s="20" t="s">
+      <c r="H111" s="17"/>
+      <c r="I111" s="17"/>
+      <c r="J111" s="17"/>
+      <c r="K111" s="17"/>
+      <c r="L111" s="17"/>
+      <c r="M111" s="17"/>
+      <c r="O111" s="17"/>
+      <c r="AMF111" s="17"/>
+      <c r="AMG111" s="17"/>
+      <c r="AMH111" s="17"/>
+      <c r="AMI111" s="17"/>
+      <c r="AMJ111" s="17"/>
+    </row>
+    <row r="112" s="17" customFormat="1" ht="12.75">
+      <c r="A112" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B112" s="20" t="s">
+      <c r="B112" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="C112" s="19" t="s">
+      <c r="C112" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D112" s="19"/>
-      <c r="E112" s="19" t="s">
+      <c r="D112" s="17"/>
+      <c r="E112" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="F112" s="19"/>
-      <c r="G112" s="19" t="s">
+      <c r="F112" s="17"/>
+      <c r="G112" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H112" s="19"/>
-      <c r="I112" s="19"/>
-      <c r="J112" s="19"/>
-      <c r="K112" s="19"/>
-      <c r="L112" s="19"/>
-      <c r="M112" s="19"/>
-      <c r="O112" s="19"/>
-      <c r="AMF112" s="19"/>
-      <c r="AMG112" s="19"/>
-      <c r="AMH112" s="19"/>
-      <c r="AMI112" s="19"/>
-      <c r="AMJ112" s="19"/>
-    </row>
-    <row r="113" s="19" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A113" s="20" t="s">
+      <c r="H112" s="17"/>
+      <c r="I112" s="17"/>
+      <c r="J112" s="17"/>
+      <c r="K112" s="17"/>
+      <c r="L112" s="17"/>
+      <c r="M112" s="17"/>
+      <c r="O112" s="17"/>
+      <c r="AMF112" s="17"/>
+      <c r="AMG112" s="17"/>
+      <c r="AMH112" s="17"/>
+      <c r="AMI112" s="17"/>
+      <c r="AMJ112" s="17"/>
+    </row>
+    <row r="113" s="17" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A113" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B113" s="20" t="s">
+      <c r="B113" s="18" t="s">
         <v>247</v>
       </c>
-      <c r="C113" s="19" t="s">
+      <c r="C113" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="D113" s="19"/>
-      <c r="E113" s="21" t="s">
+      <c r="D113" s="17"/>
+      <c r="E113" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="F113" s="19"/>
-      <c r="G113" s="19" t="s">
+      <c r="F113" s="17"/>
+      <c r="G113" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="H113" s="19"/>
-      <c r="I113" s="19"/>
-      <c r="J113" s="19"/>
-      <c r="K113" s="19"/>
-      <c r="L113" s="19"/>
-      <c r="M113" s="19"/>
-      <c r="O113" s="19"/>
-      <c r="AMF113" s="19"/>
-      <c r="AMG113" s="19"/>
-      <c r="AMH113" s="19"/>
-      <c r="AMI113" s="19"/>
-      <c r="AMJ113" s="19"/>
-    </row>
-    <row r="114" s="19" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A114" s="20" t="s">
+      <c r="H113" s="17"/>
+      <c r="I113" s="17"/>
+      <c r="J113" s="17"/>
+      <c r="K113" s="17"/>
+      <c r="L113" s="17"/>
+      <c r="M113" s="17"/>
+      <c r="O113" s="17"/>
+      <c r="AMF113" s="17"/>
+      <c r="AMG113" s="17"/>
+      <c r="AMH113" s="17"/>
+      <c r="AMI113" s="17"/>
+      <c r="AMJ113" s="17"/>
+    </row>
+    <row r="114" s="17" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A114" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B114" s="20" t="s">
+      <c r="B114" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="C114" s="19" t="s">
+      <c r="C114" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="D114" s="19"/>
-      <c r="E114" s="21" t="s">
+      <c r="D114" s="17"/>
+      <c r="E114" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="F114" s="19"/>
-      <c r="G114" s="19"/>
-      <c r="H114" s="19"/>
-      <c r="I114" s="19"/>
-      <c r="J114" s="19"/>
-      <c r="K114" s="19"/>
-      <c r="L114" s="19"/>
-      <c r="M114" s="19"/>
-      <c r="O114" s="19"/>
-      <c r="AMF114" s="19"/>
-      <c r="AMG114" s="19"/>
-      <c r="AMH114" s="19"/>
-      <c r="AMI114" s="19"/>
-      <c r="AMJ114" s="19"/>
-    </row>
-    <row r="115" s="19" customFormat="1" ht="12.75">
-      <c r="A115" s="20" t="s">
+      <c r="F114" s="17"/>
+      <c r="G114" s="17"/>
+      <c r="H114" s="17"/>
+      <c r="I114" s="17"/>
+      <c r="J114" s="17"/>
+      <c r="K114" s="17"/>
+      <c r="L114" s="17"/>
+      <c r="M114" s="17"/>
+      <c r="O114" s="17"/>
+      <c r="AMF114" s="17"/>
+      <c r="AMG114" s="17"/>
+      <c r="AMH114" s="17"/>
+      <c r="AMI114" s="17"/>
+      <c r="AMJ114" s="17"/>
+    </row>
+    <row r="115" s="17" customFormat="1" ht="12.75">
+      <c r="A115" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B115" s="20" t="s">
+      <c r="B115" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="C115" s="19" t="s">
+      <c r="C115" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="D115" s="19"/>
-      <c r="E115" s="19" t="s">
+      <c r="D115" s="17"/>
+      <c r="E115" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="F115" s="19"/>
-      <c r="G115" s="19" t="s">
+      <c r="F115" s="17"/>
+      <c r="G115" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H115" s="19"/>
-      <c r="I115" s="19"/>
-      <c r="J115" s="19"/>
-      <c r="K115" s="19"/>
-      <c r="L115" s="19"/>
-      <c r="M115" s="19"/>
-      <c r="O115" s="19"/>
-      <c r="AMF115" s="19"/>
-      <c r="AMG115" s="19"/>
-      <c r="AMH115" s="19"/>
-      <c r="AMI115" s="19"/>
-      <c r="AMJ115" s="19"/>
-    </row>
-    <row r="116" s="19" customFormat="1" ht="12.75">
-      <c r="A116" s="20" t="s">
+      <c r="H115" s="17"/>
+      <c r="I115" s="17"/>
+      <c r="J115" s="17"/>
+      <c r="K115" s="17"/>
+      <c r="L115" s="17"/>
+      <c r="M115" s="17"/>
+      <c r="O115" s="17"/>
+      <c r="AMF115" s="17"/>
+      <c r="AMG115" s="17"/>
+      <c r="AMH115" s="17"/>
+      <c r="AMI115" s="17"/>
+      <c r="AMJ115" s="17"/>
+    </row>
+    <row r="116" s="17" customFormat="1" ht="12.75">
+      <c r="A116" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B116" s="20" t="s">
+      <c r="B116" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="C116" s="19" t="s">
+      <c r="C116" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="D116" s="19"/>
-      <c r="E116" s="19" t="s">
+      <c r="D116" s="17"/>
+      <c r="E116" s="17" t="s">
         <v>256</v>
       </c>
-      <c r="F116" s="19"/>
-      <c r="G116" s="19" t="s">
+      <c r="F116" s="17"/>
+      <c r="G116" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H116" s="19"/>
-      <c r="I116" s="19"/>
-      <c r="J116" s="19"/>
-      <c r="K116" s="19"/>
-      <c r="L116" s="19"/>
-      <c r="M116" s="19"/>
-      <c r="O116" s="19"/>
-      <c r="AMF116" s="19"/>
-      <c r="AMG116" s="19"/>
-      <c r="AMH116" s="19"/>
-      <c r="AMI116" s="19"/>
-      <c r="AMJ116" s="19"/>
-    </row>
-    <row r="117" s="19" customFormat="1" ht="12.75">
-      <c r="A117" s="20" t="s">
+      <c r="H116" s="17"/>
+      <c r="I116" s="17"/>
+      <c r="J116" s="17"/>
+      <c r="K116" s="17"/>
+      <c r="L116" s="17"/>
+      <c r="M116" s="17"/>
+      <c r="O116" s="17"/>
+      <c r="AMF116" s="17"/>
+      <c r="AMG116" s="17"/>
+      <c r="AMH116" s="17"/>
+      <c r="AMI116" s="17"/>
+      <c r="AMJ116" s="17"/>
+    </row>
+    <row r="117" s="17" customFormat="1" ht="12.75">
+      <c r="A117" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B117" s="20" t="s">
+      <c r="B117" s="18" t="s">
         <v>257</v>
       </c>
-      <c r="C117" s="19" t="s">
+      <c r="C117" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="D117" s="19"/>
-      <c r="E117" s="19" t="s">
+      <c r="D117" s="17"/>
+      <c r="E117" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="F117" s="19"/>
-      <c r="G117" s="19" t="s">
+      <c r="F117" s="17"/>
+      <c r="G117" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H117" s="19"/>
-      <c r="I117" s="19"/>
-      <c r="J117" s="19"/>
-      <c r="K117" s="19"/>
-      <c r="L117" s="19"/>
-      <c r="M117" s="19"/>
-      <c r="O117" s="19"/>
-      <c r="AMF117" s="19"/>
-      <c r="AMG117" s="19"/>
-      <c r="AMH117" s="19"/>
-      <c r="AMI117" s="19"/>
-      <c r="AMJ117" s="19"/>
-    </row>
-    <row r="118" s="19" customFormat="1" ht="12.75">
-      <c r="A118" s="20" t="s">
+      <c r="H117" s="17"/>
+      <c r="I117" s="17"/>
+      <c r="J117" s="17"/>
+      <c r="K117" s="17"/>
+      <c r="L117" s="17"/>
+      <c r="M117" s="17"/>
+      <c r="O117" s="17"/>
+      <c r="AMF117" s="17"/>
+      <c r="AMG117" s="17"/>
+      <c r="AMH117" s="17"/>
+      <c r="AMI117" s="17"/>
+      <c r="AMJ117" s="17"/>
+    </row>
+    <row r="118" s="17" customFormat="1" ht="12.75">
+      <c r="A118" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B118" s="20" t="s">
+      <c r="B118" s="18" t="s">
         <v>260</v>
       </c>
-      <c r="C118" s="19" t="s">
+      <c r="C118" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="D118" s="19"/>
-      <c r="E118" s="19" t="s">
+      <c r="D118" s="17"/>
+      <c r="E118" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="F118" s="19"/>
-      <c r="G118" s="19" t="s">
+      <c r="F118" s="17"/>
+      <c r="G118" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H118" s="19"/>
-      <c r="I118" s="19"/>
-      <c r="J118" s="19"/>
-      <c r="K118" s="19"/>
-      <c r="L118" s="19"/>
-      <c r="M118" s="19"/>
-      <c r="AMF118" s="19"/>
-      <c r="AMG118" s="19"/>
-      <c r="AMH118" s="19"/>
-      <c r="AMI118" s="19"/>
-      <c r="AMJ118" s="19"/>
-    </row>
-    <row r="119" s="19" customFormat="1" ht="12.75">
-      <c r="A119" s="20" t="s">
+      <c r="H118" s="17"/>
+      <c r="I118" s="17"/>
+      <c r="J118" s="17"/>
+      <c r="K118" s="17"/>
+      <c r="L118" s="17"/>
+      <c r="M118" s="17"/>
+      <c r="AMF118" s="17"/>
+      <c r="AMG118" s="17"/>
+      <c r="AMH118" s="17"/>
+      <c r="AMI118" s="17"/>
+      <c r="AMJ118" s="17"/>
+    </row>
+    <row r="119" s="17" customFormat="1" ht="12.75">
+      <c r="A119" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B119" s="20" t="s">
+      <c r="B119" s="18" t="s">
         <v>263</v>
       </c>
-      <c r="C119" s="19" t="s">
+      <c r="C119" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="D119" s="19"/>
-      <c r="E119" s="19" t="s">
+      <c r="D119" s="17"/>
+      <c r="E119" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="F119" s="19"/>
-      <c r="G119" s="19" t="s">
+      <c r="F119" s="17"/>
+      <c r="G119" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H119" s="19"/>
-      <c r="I119" s="19"/>
-      <c r="J119" s="19"/>
-      <c r="K119" s="19"/>
-      <c r="L119" s="19"/>
-      <c r="M119" s="19"/>
-      <c r="AMF119" s="19"/>
-      <c r="AMG119" s="19"/>
-      <c r="AMH119" s="19"/>
-      <c r="AMI119" s="19"/>
-      <c r="AMJ119" s="19"/>
-    </row>
-    <row r="120" s="19" customFormat="1" ht="12.75">
-      <c r="A120" s="20" t="s">
+      <c r="H119" s="17"/>
+      <c r="I119" s="17"/>
+      <c r="J119" s="17"/>
+      <c r="K119" s="17"/>
+      <c r="L119" s="17"/>
+      <c r="M119" s="17"/>
+      <c r="AMF119" s="17"/>
+      <c r="AMG119" s="17"/>
+      <c r="AMH119" s="17"/>
+      <c r="AMI119" s="17"/>
+      <c r="AMJ119" s="17"/>
+    </row>
+    <row r="120" s="17" customFormat="1" ht="12.75">
+      <c r="A120" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B120" s="20" t="s">
+      <c r="B120" s="18" t="s">
         <v>266</v>
       </c>
-      <c r="C120" s="19" t="s">
+      <c r="C120" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="D120" s="19"/>
-      <c r="E120" s="19" t="s">
+      <c r="D120" s="17"/>
+      <c r="E120" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="F120" s="19"/>
-      <c r="G120" s="19"/>
-      <c r="H120" s="19"/>
-      <c r="I120" s="19"/>
-      <c r="J120" s="19"/>
-      <c r="K120" s="19"/>
-      <c r="L120" s="19"/>
-      <c r="M120" s="19"/>
-      <c r="AMF120" s="19"/>
-      <c r="AMG120" s="19"/>
-      <c r="AMH120" s="19"/>
-      <c r="AMI120" s="19"/>
-      <c r="AMJ120" s="19"/>
-    </row>
-    <row r="121" s="19" customFormat="1" ht="12.75">
-      <c r="A121" s="20"/>
-      <c r="B121" s="20"/>
-      <c r="C121" s="19"/>
-      <c r="D121" s="19"/>
-      <c r="E121" s="19"/>
-      <c r="F121" s="19"/>
-      <c r="G121" s="19"/>
-      <c r="H121" s="19"/>
-      <c r="I121" s="19"/>
-      <c r="J121" s="19"/>
-      <c r="K121" s="19"/>
-      <c r="L121" s="19"/>
-      <c r="M121" s="19"/>
-      <c r="AMF121" s="19"/>
-      <c r="AMG121" s="19"/>
-      <c r="AMH121" s="19"/>
-      <c r="AMI121" s="19"/>
-      <c r="AMJ121" s="19"/>
-    </row>
-    <row r="122" s="19" customFormat="1" ht="12.75">
-      <c r="A122" s="20" t="s">
+      <c r="F120" s="17"/>
+      <c r="G120" s="17"/>
+      <c r="H120" s="17"/>
+      <c r="I120" s="17"/>
+      <c r="J120" s="17"/>
+      <c r="K120" s="17"/>
+      <c r="L120" s="17"/>
+      <c r="M120" s="17"/>
+      <c r="AMF120" s="17"/>
+      <c r="AMG120" s="17"/>
+      <c r="AMH120" s="17"/>
+      <c r="AMI120" s="17"/>
+      <c r="AMJ120" s="17"/>
+    </row>
+    <row r="121" s="17" customFormat="1" ht="12.75">
+      <c r="A121" s="18"/>
+      <c r="B121" s="18"/>
+      <c r="C121" s="17"/>
+      <c r="D121" s="17"/>
+      <c r="E121" s="17"/>
+      <c r="F121" s="17"/>
+      <c r="G121" s="17"/>
+      <c r="H121" s="17"/>
+      <c r="I121" s="17"/>
+      <c r="J121" s="17"/>
+      <c r="K121" s="17"/>
+      <c r="L121" s="17"/>
+      <c r="M121" s="17"/>
+      <c r="AMF121" s="17"/>
+      <c r="AMG121" s="17"/>
+      <c r="AMH121" s="17"/>
+      <c r="AMI121" s="17"/>
+      <c r="AMJ121" s="17"/>
+    </row>
+    <row r="122" s="17" customFormat="1" ht="12.75">
+      <c r="A122" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B122" s="20" t="s">
+      <c r="B122" s="18" t="s">
         <v>269</v>
       </c>
-      <c r="C122" s="19" t="s">
+      <c r="C122" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="D122" s="19"/>
-      <c r="E122" s="19"/>
-      <c r="F122" s="19"/>
-      <c r="G122" s="19" t="s">
+      <c r="D122" s="17"/>
+      <c r="E122" s="17"/>
+      <c r="F122" s="17"/>
+      <c r="G122" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="H122" s="19"/>
-      <c r="I122" s="19"/>
-      <c r="J122" s="19"/>
-      <c r="K122" s="19"/>
-      <c r="L122" s="19"/>
-      <c r="M122" s="19"/>
-      <c r="P122" s="19"/>
-      <c r="AMF122" s="19"/>
-      <c r="AMG122" s="19"/>
-      <c r="AMH122" s="19"/>
-      <c r="AMI122" s="19"/>
-      <c r="AMJ122" s="19"/>
-    </row>
-    <row r="123" s="19" customFormat="1" ht="12.75">
-      <c r="A123" s="20" t="s">
+      <c r="H122" s="17"/>
+      <c r="I122" s="17"/>
+      <c r="J122" s="17"/>
+      <c r="K122" s="17"/>
+      <c r="L122" s="17"/>
+      <c r="M122" s="17"/>
+      <c r="P122" s="17"/>
+      <c r="AMF122" s="17"/>
+      <c r="AMG122" s="17"/>
+      <c r="AMH122" s="17"/>
+      <c r="AMI122" s="17"/>
+      <c r="AMJ122" s="17"/>
+    </row>
+    <row r="123" s="17" customFormat="1" ht="12.75">
+      <c r="A123" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="B123" s="20" t="s">
+      <c r="B123" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="C123" s="19" t="s">
+      <c r="C123" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D123" s="19"/>
-      <c r="E123" s="19"/>
-      <c r="F123" s="19"/>
-      <c r="G123" s="19"/>
-      <c r="H123" s="19"/>
-      <c r="I123" s="19"/>
-      <c r="J123" s="19"/>
-      <c r="K123" s="19"/>
-      <c r="L123" s="19"/>
-      <c r="M123" s="19" t="s">
+      <c r="D123" s="17"/>
+      <c r="E123" s="17"/>
+      <c r="F123" s="17"/>
+      <c r="G123" s="17"/>
+      <c r="H123" s="17"/>
+      <c r="I123" s="17"/>
+      <c r="J123" s="17"/>
+      <c r="K123" s="17"/>
+      <c r="L123" s="17"/>
+      <c r="M123" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="AMF123" s="19"/>
-      <c r="AMG123" s="19"/>
-      <c r="AMH123" s="19"/>
-      <c r="AMI123" s="19"/>
-      <c r="AMJ123" s="19"/>
-    </row>
-    <row r="124" s="19" customFormat="1" ht="12.75">
-      <c r="A124" s="20" t="s">
+      <c r="AMF123" s="17"/>
+      <c r="AMG123" s="17"/>
+      <c r="AMH123" s="17"/>
+      <c r="AMI123" s="17"/>
+      <c r="AMJ123" s="17"/>
+    </row>
+    <row r="124" s="17" customFormat="1" ht="12.75">
+      <c r="A124" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B124" s="20" t="s">
+      <c r="B124" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="C124" s="19"/>
-      <c r="D124" s="19"/>
-      <c r="E124" s="19"/>
-      <c r="F124" s="19" t="s">
+      <c r="C124" s="17"/>
+      <c r="D124" s="17"/>
+      <c r="E124" s="17"/>
+      <c r="F124" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="G124" s="19"/>
-      <c r="H124" s="19"/>
-      <c r="I124" s="19"/>
-      <c r="J124" s="19"/>
-      <c r="K124" s="19"/>
-      <c r="L124" s="19"/>
-      <c r="M124" s="19"/>
-      <c r="AMF124" s="19"/>
-      <c r="AMG124" s="19"/>
-      <c r="AMH124" s="19"/>
-      <c r="AMI124" s="19"/>
-      <c r="AMJ124" s="19"/>
-    </row>
-    <row r="125" s="19" customFormat="1" ht="12.75">
-      <c r="A125" s="20" t="s">
+      <c r="G124" s="17"/>
+      <c r="H124" s="17"/>
+      <c r="I124" s="17"/>
+      <c r="J124" s="17"/>
+      <c r="K124" s="17"/>
+      <c r="L124" s="17"/>
+      <c r="M124" s="17"/>
+      <c r="AMF124" s="17"/>
+      <c r="AMG124" s="17"/>
+      <c r="AMH124" s="17"/>
+      <c r="AMI124" s="17"/>
+      <c r="AMJ124" s="17"/>
+    </row>
+    <row r="125" s="17" customFormat="1" ht="12.75">
+      <c r="A125" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B125" s="20" t="s">
+      <c r="B125" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="C125" s="19"/>
-      <c r="D125" s="19"/>
-      <c r="E125" s="19"/>
-      <c r="F125" s="19" t="s">
+      <c r="C125" s="17"/>
+      <c r="D125" s="17"/>
+      <c r="E125" s="17"/>
+      <c r="F125" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="G125" s="19"/>
-      <c r="H125" s="19"/>
-      <c r="I125" s="19"/>
-      <c r="J125" s="19"/>
-      <c r="K125" s="19"/>
-      <c r="L125" s="19"/>
-      <c r="M125" s="19"/>
-      <c r="AMF125" s="19"/>
-      <c r="AMG125" s="19"/>
-      <c r="AMH125" s="19"/>
-      <c r="AMI125" s="19"/>
-      <c r="AMJ125" s="19"/>
-    </row>
-    <row r="126" s="19" customFormat="1" ht="12.75">
-      <c r="A126" s="20" t="s">
+      <c r="G125" s="17"/>
+      <c r="H125" s="17"/>
+      <c r="I125" s="17"/>
+      <c r="J125" s="17"/>
+      <c r="K125" s="17"/>
+      <c r="L125" s="17"/>
+      <c r="M125" s="17"/>
+      <c r="AMF125" s="17"/>
+      <c r="AMG125" s="17"/>
+      <c r="AMH125" s="17"/>
+      <c r="AMI125" s="17"/>
+      <c r="AMJ125" s="17"/>
+    </row>
+    <row r="126" s="17" customFormat="1" ht="12.75">
+      <c r="A126" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B126" s="20" t="s">
+      <c r="B126" s="18" t="s">
         <v>278</v>
       </c>
-      <c r="C126" s="19"/>
-      <c r="D126" s="19"/>
-      <c r="E126" s="19"/>
-      <c r="F126" s="19" t="s">
+      <c r="C126" s="17"/>
+      <c r="D126" s="17"/>
+      <c r="E126" s="17"/>
+      <c r="F126" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="G126" s="19"/>
-      <c r="H126" s="19"/>
-      <c r="I126" s="19"/>
-      <c r="J126" s="19"/>
-      <c r="K126" s="19"/>
-      <c r="L126" s="19"/>
-      <c r="M126" s="19"/>
-      <c r="AMF126" s="19"/>
-      <c r="AMG126" s="19"/>
-      <c r="AMH126" s="19"/>
-      <c r="AMI126" s="19"/>
-      <c r="AMJ126" s="19"/>
-    </row>
-    <row r="127" s="19" customFormat="1" ht="12.75">
+      <c r="G126" s="17"/>
+      <c r="H126" s="17"/>
+      <c r="I126" s="17"/>
+      <c r="J126" s="17"/>
+      <c r="K126" s="17"/>
+      <c r="L126" s="17"/>
+      <c r="M126" s="17"/>
+      <c r="AMF126" s="17"/>
+      <c r="AMG126" s="17"/>
+      <c r="AMH126" s="17"/>
+      <c r="AMI126" s="17"/>
+      <c r="AMJ126" s="17"/>
+    </row>
+    <row r="127" s="17" customFormat="1" ht="12.75">
       <c r="A127" s="20" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="B127" s="20" t="s">
         <v>280</v>
       </c>
-      <c r="C127" s="19" t="s">
+      <c r="C127" s="17"/>
+      <c r="D127" s="17"/>
+      <c r="E127" s="17"/>
+      <c r="F127" s="21" t="s">
         <v>281</v>
       </c>
-      <c r="D127" s="19"/>
-      <c r="E127" s="19"/>
-      <c r="F127" s="19"/>
-      <c r="G127" s="19" t="s">
+      <c r="G127" s="17"/>
+      <c r="H127" s="17"/>
+      <c r="I127" s="17"/>
+      <c r="J127" s="17"/>
+      <c r="K127" s="17"/>
+      <c r="L127" s="17"/>
+      <c r="M127" s="17"/>
+      <c r="AMF127" s="17"/>
+      <c r="AMG127" s="17"/>
+      <c r="AMH127" s="17"/>
+      <c r="AMI127" s="17"/>
+      <c r="AMJ127" s="17"/>
+    </row>
+    <row r="128" s="17" customFormat="1" ht="12.75">
+      <c r="A128" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B128" s="20" t="s">
         <v>282</v>
       </c>
-      <c r="H127" s="19"/>
-      <c r="I127" s="19"/>
-      <c r="J127" s="19"/>
-      <c r="K127" s="19"/>
-      <c r="L127" s="19"/>
-      <c r="M127" s="19"/>
-      <c r="AMF127" s="19"/>
-      <c r="AMG127" s="19"/>
-      <c r="AMH127" s="19"/>
-      <c r="AMI127" s="19"/>
-      <c r="AMJ127" s="19"/>
-    </row>
-    <row r="128" s="19" customFormat="1" ht="12.75">
-      <c r="A128" s="20" t="s">
+      <c r="C128" s="17"/>
+      <c r="D128" s="17"/>
+      <c r="E128" s="17"/>
+      <c r="F128" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="G128" s="17"/>
+      <c r="H128" s="17"/>
+      <c r="I128" s="17"/>
+      <c r="J128" s="17"/>
+      <c r="K128" s="17"/>
+      <c r="L128" s="17"/>
+      <c r="M128" s="17"/>
+      <c r="AMF128" s="17"/>
+      <c r="AMG128" s="17"/>
+      <c r="AMH128" s="17"/>
+      <c r="AMI128" s="17"/>
+      <c r="AMJ128" s="17"/>
+    </row>
+    <row r="129" s="17" customFormat="1" ht="12.75">
+      <c r="A129" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B129" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="C129" s="17"/>
+      <c r="D129" s="17"/>
+      <c r="E129" s="17"/>
+      <c r="F129" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="G129" s="17"/>
+      <c r="H129" s="17"/>
+      <c r="I129" s="17"/>
+      <c r="J129" s="17"/>
+      <c r="K129" s="17"/>
+      <c r="L129" s="17"/>
+      <c r="M129" s="17"/>
+      <c r="AMF129" s="17"/>
+      <c r="AMG129" s="17"/>
+      <c r="AMH129" s="17"/>
+      <c r="AMI129" s="17"/>
+      <c r="AMJ129" s="17"/>
+    </row>
+    <row r="130" s="17" customFormat="1" ht="12.75">
+      <c r="A130" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B130" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="C130" s="17"/>
+      <c r="D130" s="17"/>
+      <c r="E130" s="17"/>
+      <c r="F130" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="G130" s="17"/>
+      <c r="H130" s="17"/>
+      <c r="I130" s="17"/>
+      <c r="J130" s="17"/>
+      <c r="K130" s="17"/>
+      <c r="L130" s="17"/>
+      <c r="M130" s="17"/>
+      <c r="AMF130" s="17"/>
+      <c r="AMG130" s="17"/>
+      <c r="AMH130" s="17"/>
+      <c r="AMI130" s="17"/>
+      <c r="AMJ130" s="17"/>
+    </row>
+    <row r="131" s="17" customFormat="1" ht="12.75">
+      <c r="A131" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B131" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="C131" s="17"/>
+      <c r="D131" s="17"/>
+      <c r="E131" s="17"/>
+      <c r="F131" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="G131" s="17"/>
+      <c r="H131" s="17"/>
+      <c r="I131" s="17"/>
+      <c r="J131" s="17"/>
+      <c r="K131" s="17"/>
+      <c r="L131" s="17"/>
+      <c r="M131" s="17"/>
+      <c r="AMF131" s="17"/>
+      <c r="AMG131" s="17"/>
+      <c r="AMH131" s="17"/>
+      <c r="AMI131" s="17"/>
+      <c r="AMJ131" s="17"/>
+    </row>
+    <row r="132" s="17" customFormat="1" ht="12.75">
+      <c r="A132" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B132" s="20" t="s">
+        <v>290</v>
+      </c>
+      <c r="C132" s="17"/>
+      <c r="D132" s="17"/>
+      <c r="E132" s="17"/>
+      <c r="F132" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="G132" s="17"/>
+      <c r="H132" s="17"/>
+      <c r="I132" s="17"/>
+      <c r="J132" s="17"/>
+      <c r="K132" s="17"/>
+      <c r="L132" s="17"/>
+      <c r="M132" s="17"/>
+      <c r="AMF132" s="17"/>
+      <c r="AMG132" s="17"/>
+      <c r="AMH132" s="17"/>
+      <c r="AMI132" s="17"/>
+      <c r="AMJ132" s="17"/>
+    </row>
+    <row r="133" s="17" customFormat="1" ht="12.75">
+      <c r="A133" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B133" s="20" t="s">
+        <v>292</v>
+      </c>
+      <c r="C133" s="17"/>
+      <c r="D133" s="17"/>
+      <c r="E133" s="17"/>
+      <c r="F133" s="21" t="s">
+        <v>293</v>
+      </c>
+      <c r="G133" s="17"/>
+      <c r="H133" s="17"/>
+      <c r="I133" s="17"/>
+      <c r="J133" s="17"/>
+      <c r="K133" s="17"/>
+      <c r="L133" s="17"/>
+      <c r="M133" s="17"/>
+      <c r="AMF133" s="17"/>
+      <c r="AMG133" s="17"/>
+      <c r="AMH133" s="17"/>
+      <c r="AMI133" s="17"/>
+      <c r="AMJ133" s="17"/>
+    </row>
+    <row r="134" s="17" customFormat="1" ht="12.75">
+      <c r="A134" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B134" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="C134" s="17"/>
+      <c r="D134" s="17"/>
+      <c r="E134" s="17"/>
+      <c r="F134" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="G134" s="17"/>
+      <c r="H134" s="17"/>
+      <c r="I134" s="17"/>
+      <c r="J134" s="17"/>
+      <c r="K134" s="17"/>
+      <c r="L134" s="17"/>
+      <c r="M134" s="17"/>
+      <c r="AMF134" s="17"/>
+      <c r="AMG134" s="17"/>
+      <c r="AMH134" s="17"/>
+      <c r="AMI134" s="17"/>
+      <c r="AMJ134" s="17"/>
+    </row>
+    <row r="135" s="17" customFormat="1" ht="12.75">
+      <c r="A135" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B135" s="20" t="s">
+        <v>296</v>
+      </c>
+      <c r="C135" s="17"/>
+      <c r="D135" s="17"/>
+      <c r="E135" s="17"/>
+      <c r="F135" s="21" t="s">
+        <v>297</v>
+      </c>
+      <c r="G135" s="17"/>
+      <c r="H135" s="17"/>
+      <c r="I135" s="17"/>
+      <c r="J135" s="17"/>
+      <c r="K135" s="17"/>
+      <c r="L135" s="17"/>
+      <c r="M135" s="17"/>
+      <c r="AMF135" s="17"/>
+      <c r="AMG135" s="17"/>
+      <c r="AMH135" s="17"/>
+      <c r="AMI135" s="17"/>
+      <c r="AMJ135" s="17"/>
+    </row>
+    <row r="136" s="17" customFormat="1" ht="12.75">
+      <c r="A136" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B136" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="C136" s="17"/>
+      <c r="D136" s="17"/>
+      <c r="E136" s="17"/>
+      <c r="F136" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="G136" s="17"/>
+      <c r="H136" s="17"/>
+      <c r="I136" s="17"/>
+      <c r="J136" s="17"/>
+      <c r="K136" s="17"/>
+      <c r="L136" s="17"/>
+      <c r="M136" s="17"/>
+      <c r="AMF136" s="17"/>
+      <c r="AMG136" s="17"/>
+      <c r="AMH136" s="17"/>
+      <c r="AMI136" s="17"/>
+      <c r="AMJ136" s="17"/>
+    </row>
+    <row r="137" s="17" customFormat="1" ht="12.75">
+      <c r="A137" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B128" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="C128" s="19" t="s">
-        <v>284</v>
-      </c>
-      <c r="D128" s="19"/>
-      <c r="E128" s="19"/>
-      <c r="F128" s="19"/>
-      <c r="G128" s="19" t="s">
+      <c r="B137" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="C137" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="D137" s="17"/>
+      <c r="E137" s="17"/>
+      <c r="F137" s="17"/>
+      <c r="G137" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="H137" s="17"/>
+      <c r="I137" s="17"/>
+      <c r="J137" s="17"/>
+      <c r="K137" s="17"/>
+      <c r="L137" s="17"/>
+      <c r="M137" s="17"/>
+      <c r="AMF137" s="17"/>
+      <c r="AMG137" s="17"/>
+      <c r="AMH137" s="17"/>
+      <c r="AMI137" s="17"/>
+      <c r="AMJ137" s="17"/>
+    </row>
+    <row r="138" s="17" customFormat="1" ht="12.75">
+      <c r="A138" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B138" s="18" t="s">
+        <v>303</v>
+      </c>
+      <c r="C138" s="17" t="s">
+        <v>304</v>
+      </c>
+      <c r="D138" s="17"/>
+      <c r="E138" s="17"/>
+      <c r="F138" s="17"/>
+      <c r="G138" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H128" s="19"/>
-      <c r="I128" s="19"/>
-      <c r="J128" s="19"/>
-      <c r="K128" s="19"/>
-      <c r="L128" s="19"/>
-      <c r="M128" s="19"/>
-      <c r="AMF128" s="19"/>
-      <c r="AMG128" s="19"/>
-      <c r="AMH128" s="19"/>
-      <c r="AMI128" s="19"/>
-      <c r="AMJ128" s="19"/>
-    </row>
-    <row r="129" s="19" customFormat="1" ht="12.75">
-      <c r="A129" s="20" t="s">
+      <c r="H138" s="17"/>
+      <c r="I138" s="17"/>
+      <c r="J138" s="17"/>
+      <c r="K138" s="17"/>
+      <c r="L138" s="17"/>
+      <c r="M138" s="17"/>
+      <c r="AMF138" s="17"/>
+      <c r="AMG138" s="17"/>
+      <c r="AMH138" s="17"/>
+      <c r="AMI138" s="17"/>
+      <c r="AMJ138" s="17"/>
+    </row>
+    <row r="139" s="17" customFormat="1" ht="12.75">
+      <c r="A139" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B129" s="20" t="s">
-        <v>285</v>
-      </c>
-      <c r="C129" s="19" t="s">
-        <v>286</v>
-      </c>
-      <c r="D129" s="19"/>
-      <c r="E129" s="19"/>
-      <c r="F129" s="19"/>
-      <c r="G129" s="19" t="s">
+      <c r="B139" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="C139" s="17" t="s">
+        <v>306</v>
+      </c>
+      <c r="D139" s="17"/>
+      <c r="E139" s="17"/>
+      <c r="F139" s="17"/>
+      <c r="G139" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H129" s="19"/>
-      <c r="I129" s="19"/>
-      <c r="J129" s="19"/>
-      <c r="K129" s="19"/>
-      <c r="L129" s="19"/>
-      <c r="M129" s="19"/>
-      <c r="AMF129" s="19"/>
-      <c r="AMG129" s="19"/>
-      <c r="AMH129" s="19"/>
-      <c r="AMI129" s="19"/>
-      <c r="AMJ129" s="19"/>
-    </row>
-    <row r="130" s="19" customFormat="1" ht="12.75">
-      <c r="A130" s="22" t="s">
+      <c r="H139" s="17"/>
+      <c r="I139" s="17"/>
+      <c r="J139" s="17"/>
+      <c r="K139" s="17"/>
+      <c r="L139" s="17"/>
+      <c r="M139" s="17"/>
+      <c r="AMF139" s="17"/>
+      <c r="AMG139" s="17"/>
+      <c r="AMH139" s="17"/>
+      <c r="AMI139" s="17"/>
+      <c r="AMJ139" s="17"/>
+    </row>
+    <row r="140" s="17" customFormat="1" ht="12.75">
+      <c r="A140" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B130" s="22" t="s">
+      <c r="B140" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="C130" s="23" t="s">
+      <c r="C140" s="23" t="s">
         <v>235</v>
       </c>
-      <c r="D130" s="19"/>
-      <c r="E130" s="19" t="s">
-        <v>287</v>
-      </c>
-      <c r="F130" s="19"/>
-      <c r="G130" s="19" t="s">
-        <v>288</v>
-      </c>
-      <c r="H130" s="19"/>
-      <c r="I130" s="19"/>
-      <c r="J130" s="19"/>
-      <c r="K130" s="19"/>
-      <c r="L130" s="19"/>
-      <c r="M130" s="19"/>
-      <c r="AMF130" s="19"/>
-      <c r="AMG130" s="19"/>
-      <c r="AMH130" s="19"/>
-      <c r="AMI130" s="19"/>
-      <c r="AMJ130" s="19"/>
-    </row>
-    <row r="131" s="19" customFormat="1" ht="12.75">
-      <c r="A131" s="22" t="s">
+      <c r="D140" s="17"/>
+      <c r="E140" s="21" t="s">
+        <v>307</v>
+      </c>
+      <c r="F140" s="17"/>
+      <c r="G140" s="17" t="s">
+        <v>308</v>
+      </c>
+      <c r="H140" s="17"/>
+      <c r="I140" s="17"/>
+      <c r="J140" s="17"/>
+      <c r="K140" s="17"/>
+      <c r="L140" s="17"/>
+      <c r="M140" s="17"/>
+      <c r="AMF140" s="17"/>
+      <c r="AMG140" s="17"/>
+      <c r="AMH140" s="17"/>
+      <c r="AMI140" s="17"/>
+      <c r="AMJ140" s="17"/>
+    </row>
+    <row r="141" s="17" customFormat="1" ht="12.75">
+      <c r="A141" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B131" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="C131" s="19" t="s">
+      <c r="B141" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="C141" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="D131" s="19"/>
-      <c r="E131" s="19" t="s">
-        <v>290</v>
-      </c>
-      <c r="F131" s="19"/>
-      <c r="G131" s="19" t="s">
+      <c r="D141" s="17"/>
+      <c r="E141" s="21" t="s">
+        <v>310</v>
+      </c>
+      <c r="F141" s="17"/>
+      <c r="G141" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H131" s="19"/>
-      <c r="I131" s="19"/>
-      <c r="J131" s="19"/>
-      <c r="K131" s="19"/>
-      <c r="L131" s="19"/>
-      <c r="M131" s="19"/>
-      <c r="AMF131" s="19"/>
-      <c r="AMG131" s="19"/>
-      <c r="AMH131" s="19"/>
-      <c r="AMI131" s="19"/>
-      <c r="AMJ131" s="19"/>
-    </row>
-    <row r="132" s="19" customFormat="1" ht="12.75">
-      <c r="A132" s="22" t="s">
+      <c r="H141" s="17"/>
+      <c r="I141" s="17"/>
+      <c r="J141" s="17"/>
+      <c r="K141" s="17"/>
+      <c r="L141" s="17"/>
+      <c r="M141" s="17"/>
+      <c r="AMF141" s="17"/>
+      <c r="AMG141" s="17"/>
+      <c r="AMH141" s="17"/>
+      <c r="AMI141" s="17"/>
+      <c r="AMJ141" s="17"/>
+    </row>
+    <row r="142" s="17" customFormat="1" ht="12.75">
+      <c r="A142" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B132" s="20" t="s">
-        <v>291</v>
-      </c>
-      <c r="C132" s="19" t="s">
+      <c r="B142" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="C142" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D132" s="19"/>
-      <c r="E132" s="19" t="s">
-        <v>292</v>
-      </c>
-      <c r="F132" s="19"/>
-      <c r="G132" s="19" t="s">
+      <c r="D142" s="17"/>
+      <c r="E142" s="21" t="s">
+        <v>312</v>
+      </c>
+      <c r="F142" s="17"/>
+      <c r="G142" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H132" s="19"/>
-      <c r="I132" s="19"/>
-      <c r="J132" s="19"/>
-      <c r="K132" s="19"/>
-      <c r="L132" s="19"/>
-      <c r="M132" s="19"/>
-      <c r="AMF132" s="19"/>
-      <c r="AMG132" s="19"/>
-      <c r="AMH132" s="19"/>
-      <c r="AMI132" s="19"/>
-      <c r="AMJ132" s="19"/>
-    </row>
-    <row r="133" s="19" customFormat="1" ht="12.75">
-      <c r="A133" s="22" t="s">
+      <c r="H142" s="17"/>
+      <c r="I142" s="17"/>
+      <c r="J142" s="17"/>
+      <c r="K142" s="17"/>
+      <c r="L142" s="17"/>
+      <c r="M142" s="17"/>
+      <c r="AMF142" s="17"/>
+      <c r="AMG142" s="17"/>
+      <c r="AMH142" s="17"/>
+      <c r="AMI142" s="17"/>
+      <c r="AMJ142" s="17"/>
+    </row>
+    <row r="143" s="17" customFormat="1" ht="12.75">
+      <c r="A143" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B133" s="20" t="s">
-        <v>293</v>
-      </c>
-      <c r="C133" s="19" t="s">
+      <c r="B143" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="C143" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="D133" s="19"/>
-      <c r="E133" s="19" t="s">
-        <v>294</v>
-      </c>
-      <c r="F133" s="19"/>
-      <c r="G133" s="19" t="s">
+      <c r="D143" s="17"/>
+      <c r="E143" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="F143" s="17"/>
+      <c r="G143" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H133" s="19"/>
-      <c r="I133" s="19"/>
-      <c r="J133" s="19"/>
-      <c r="K133" s="19"/>
-      <c r="L133" s="19"/>
-      <c r="M133" s="19"/>
-      <c r="AMF133" s="19"/>
-      <c r="AMG133" s="19"/>
-      <c r="AMH133" s="19"/>
-      <c r="AMI133" s="19"/>
-      <c r="AMJ133" s="19"/>
-    </row>
-    <row r="134" s="19" customFormat="1" ht="12.75">
-      <c r="A134" s="22" t="s">
+      <c r="H143" s="17"/>
+      <c r="I143" s="17"/>
+      <c r="J143" s="17"/>
+      <c r="K143" s="17"/>
+      <c r="L143" s="17"/>
+      <c r="M143" s="17"/>
+      <c r="AMF143" s="17"/>
+      <c r="AMG143" s="17"/>
+      <c r="AMH143" s="17"/>
+      <c r="AMI143" s="17"/>
+      <c r="AMJ143" s="17"/>
+    </row>
+    <row r="144" s="17" customFormat="1" ht="12.75">
+      <c r="A144" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B134" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="C134" s="19" t="s">
+      <c r="B144" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="C144" s="17" t="s">
         <v>155</v>
       </c>
-      <c r="D134" s="19"/>
-      <c r="E134" s="19" t="s">
-        <v>296</v>
-      </c>
-      <c r="F134" s="19"/>
-      <c r="G134" s="19" t="s">
+      <c r="D144" s="17"/>
+      <c r="E144" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="F144" s="17"/>
+      <c r="G144" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H134" s="19"/>
-      <c r="I134" s="19"/>
-      <c r="J134" s="19"/>
-      <c r="K134" s="19"/>
-      <c r="L134" s="19"/>
-      <c r="M134" s="19"/>
-      <c r="AMF134" s="19"/>
-      <c r="AMG134" s="19"/>
-      <c r="AMH134" s="19"/>
-      <c r="AMI134" s="19"/>
-      <c r="AMJ134" s="19"/>
-    </row>
-    <row r="135" s="19" customFormat="1" ht="12.75">
-      <c r="A135" s="22" t="s">
+      <c r="H144" s="17"/>
+      <c r="I144" s="17"/>
+      <c r="J144" s="17"/>
+      <c r="K144" s="17"/>
+      <c r="L144" s="17"/>
+      <c r="M144" s="17"/>
+      <c r="AMF144" s="17"/>
+      <c r="AMG144" s="17"/>
+      <c r="AMH144" s="17"/>
+      <c r="AMI144" s="17"/>
+      <c r="AMJ144" s="17"/>
+    </row>
+    <row r="145" s="17" customFormat="1" ht="12.75">
+      <c r="A145" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B135" s="20" t="s">
-        <v>297</v>
-      </c>
-      <c r="C135" s="19" t="s">
+      <c r="B145" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="C145" s="17" t="s">
         <v>157</v>
       </c>
-      <c r="D135" s="19"/>
-      <c r="E135" s="19" t="s">
-        <v>298</v>
-      </c>
-      <c r="F135" s="19"/>
-      <c r="G135" s="19" t="s">
+      <c r="D145" s="17"/>
+      <c r="E145" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="F145" s="17"/>
+      <c r="G145" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H135" s="19"/>
-      <c r="I135" s="19"/>
-      <c r="J135" s="19"/>
-      <c r="K135" s="19"/>
-      <c r="L135" s="19"/>
-      <c r="M135" s="19"/>
-      <c r="AMF135" s="19"/>
-      <c r="AMG135" s="19"/>
-      <c r="AMH135" s="19"/>
-      <c r="AMI135" s="19"/>
-      <c r="AMJ135" s="19"/>
-    </row>
-    <row r="136" s="19" customFormat="1" ht="12.75">
-      <c r="A136" s="22" t="s">
+      <c r="H145" s="17"/>
+      <c r="I145" s="17"/>
+      <c r="J145" s="17"/>
+      <c r="K145" s="17"/>
+      <c r="L145" s="17"/>
+      <c r="M145" s="17"/>
+      <c r="AMF145" s="17"/>
+      <c r="AMG145" s="17"/>
+      <c r="AMH145" s="17"/>
+      <c r="AMI145" s="17"/>
+      <c r="AMJ145" s="17"/>
+    </row>
+    <row r="146" s="17" customFormat="1" ht="12.75">
+      <c r="A146" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B136" s="20" t="s">
-        <v>299</v>
-      </c>
-      <c r="C136" s="19" t="s">
+      <c r="B146" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="C146" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="D136" s="19"/>
-      <c r="E136" s="19" t="s">
-        <v>300</v>
-      </c>
-      <c r="F136" s="19"/>
-      <c r="G136" s="19" t="s">
+      <c r="D146" s="17"/>
+      <c r="E146" s="21" t="s">
+        <v>320</v>
+      </c>
+      <c r="F146" s="17"/>
+      <c r="G146" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H136" s="19"/>
-      <c r="I136" s="19"/>
-      <c r="J136" s="19"/>
-      <c r="K136" s="19"/>
-      <c r="L136" s="19"/>
-      <c r="M136" s="19"/>
-      <c r="AMF136" s="19"/>
-      <c r="AMG136" s="19"/>
-      <c r="AMH136" s="19"/>
-      <c r="AMI136" s="19"/>
-      <c r="AMJ136" s="19"/>
-    </row>
-    <row r="137" s="19" customFormat="1" ht="12.75">
-      <c r="A137" s="22" t="s">
+      <c r="H146" s="17"/>
+      <c r="I146" s="17"/>
+      <c r="J146" s="17"/>
+      <c r="K146" s="17"/>
+      <c r="L146" s="17"/>
+      <c r="M146" s="17"/>
+      <c r="AMF146" s="17"/>
+      <c r="AMG146" s="17"/>
+      <c r="AMH146" s="17"/>
+      <c r="AMI146" s="17"/>
+      <c r="AMJ146" s="17"/>
+    </row>
+    <row r="147" s="17" customFormat="1" ht="12.75">
+      <c r="A147" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B137" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="C137" s="19" t="s">
+      <c r="B147" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="C147" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="D137" s="19"/>
-      <c r="E137" s="19" t="s">
-        <v>302</v>
-      </c>
-      <c r="F137" s="19"/>
-      <c r="G137" s="19" t="s">
+      <c r="D147" s="17"/>
+      <c r="E147" s="21" t="s">
+        <v>322</v>
+      </c>
+      <c r="F147" s="17"/>
+      <c r="G147" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H137" s="19"/>
-      <c r="I137" s="19"/>
-      <c r="J137" s="19"/>
-      <c r="K137" s="19"/>
-      <c r="L137" s="19"/>
-      <c r="M137" s="19"/>
-      <c r="AMF137" s="19"/>
-      <c r="AMG137" s="19"/>
-      <c r="AMH137" s="19"/>
-      <c r="AMI137" s="19"/>
-      <c r="AMJ137" s="19"/>
-    </row>
-    <row r="138" s="19" customFormat="1" ht="12.75">
-      <c r="A138" s="22" t="s">
+      <c r="H147" s="17"/>
+      <c r="I147" s="17"/>
+      <c r="J147" s="17"/>
+      <c r="K147" s="17"/>
+      <c r="L147" s="17"/>
+      <c r="M147" s="17"/>
+      <c r="AMF147" s="17"/>
+      <c r="AMG147" s="17"/>
+      <c r="AMH147" s="17"/>
+      <c r="AMI147" s="17"/>
+      <c r="AMJ147" s="17"/>
+    </row>
+    <row r="148" s="17" customFormat="1" ht="12.75">
+      <c r="A148" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B138" s="20" t="s">
-        <v>303</v>
-      </c>
-      <c r="C138" s="19" t="s">
+      <c r="B148" s="18" t="s">
+        <v>323</v>
+      </c>
+      <c r="C148" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D138" s="19"/>
-      <c r="E138" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="F138" s="19"/>
-      <c r="G138" s="19" t="s">
+      <c r="D148" s="17"/>
+      <c r="E148" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="F148" s="17"/>
+      <c r="G148" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H138" s="19"/>
-      <c r="I138" s="19"/>
-      <c r="J138" s="19"/>
-      <c r="K138" s="19"/>
-      <c r="L138" s="19"/>
-      <c r="M138" s="19"/>
-      <c r="AMF138" s="19"/>
-      <c r="AMG138" s="19"/>
-      <c r="AMH138" s="19"/>
-      <c r="AMI138" s="19"/>
-      <c r="AMJ138" s="19"/>
-    </row>
-    <row r="139" s="19" customFormat="1" ht="12.75">
-      <c r="A139" s="22" t="s">
+      <c r="H148" s="17"/>
+      <c r="I148" s="17"/>
+      <c r="J148" s="17"/>
+      <c r="K148" s="17"/>
+      <c r="L148" s="17"/>
+      <c r="M148" s="17"/>
+      <c r="AMF148" s="17"/>
+      <c r="AMG148" s="17"/>
+      <c r="AMH148" s="17"/>
+      <c r="AMI148" s="17"/>
+      <c r="AMJ148" s="17"/>
+    </row>
+    <row r="149" s="17" customFormat="1" ht="12.75">
+      <c r="A149" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B139" s="20" t="s">
-        <v>305</v>
-      </c>
-      <c r="C139" s="19" t="s">
+      <c r="B149" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="C149" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="D139" s="19"/>
-      <c r="E139" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="F139" s="19"/>
-      <c r="G139" s="19" t="s">
+      <c r="D149" s="17"/>
+      <c r="E149" s="21" t="s">
+        <v>326</v>
+      </c>
+      <c r="F149" s="17"/>
+      <c r="G149" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H139" s="19"/>
-      <c r="I139" s="19"/>
-      <c r="J139" s="19"/>
-      <c r="K139" s="19"/>
-      <c r="L139" s="19"/>
-      <c r="M139" s="19"/>
-      <c r="AMF139" s="19"/>
-      <c r="AMG139" s="19"/>
-      <c r="AMH139" s="19"/>
-      <c r="AMI139" s="19"/>
-      <c r="AMJ139" s="19"/>
-    </row>
-    <row r="140" s="19" customFormat="1" ht="12.75">
-      <c r="A140" s="20" t="s">
+      <c r="H149" s="17"/>
+      <c r="I149" s="17"/>
+      <c r="J149" s="17"/>
+      <c r="K149" s="17"/>
+      <c r="L149" s="17"/>
+      <c r="M149" s="17"/>
+      <c r="AMF149" s="17"/>
+      <c r="AMG149" s="17"/>
+      <c r="AMH149" s="17"/>
+      <c r="AMI149" s="17"/>
+      <c r="AMJ149" s="17"/>
+    </row>
+    <row r="150" s="17" customFormat="1" ht="12.75">
+      <c r="A150" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="B140" s="20" t="s">
+      <c r="B150" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="C140" s="19"/>
-      <c r="D140" s="19"/>
-      <c r="E140" s="19"/>
-      <c r="F140" s="19"/>
-      <c r="G140" s="19"/>
-      <c r="H140" s="19"/>
-      <c r="I140" s="19"/>
-      <c r="J140" s="19"/>
-      <c r="K140" s="19"/>
-      <c r="L140" s="19"/>
-      <c r="M140" s="19"/>
-      <c r="AMF140" s="19"/>
-      <c r="AMG140" s="19"/>
-      <c r="AMH140" s="19"/>
-      <c r="AMI140" s="19"/>
-      <c r="AMJ140" s="19"/>
-    </row>
-    <row r="141" s="0" customFormat="1" ht="12.75">
-      <c r="E141" s="6"/>
-      <c r="G141" s="6"/>
-    </row>
-    <row r="142" s="19" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A142" s="20" t="s">
+      <c r="C150" s="17"/>
+      <c r="D150" s="17"/>
+      <c r="E150" s="17"/>
+      <c r="F150" s="17"/>
+      <c r="G150" s="17"/>
+      <c r="H150" s="17"/>
+      <c r="I150" s="17"/>
+      <c r="J150" s="17"/>
+      <c r="K150" s="17"/>
+      <c r="L150" s="17"/>
+      <c r="M150" s="17"/>
+      <c r="AMF150" s="17"/>
+      <c r="AMG150" s="17"/>
+      <c r="AMH150" s="17"/>
+      <c r="AMI150" s="17"/>
+      <c r="AMJ150" s="17"/>
+    </row>
+    <row r="151" s="0" customFormat="1" ht="12.75">
+      <c r="E151" s="6"/>
+      <c r="G151" s="6"/>
+    </row>
+    <row r="152" s="17" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A152" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B142" s="20" t="s">
-        <v>307</v>
-      </c>
-      <c r="C142" s="19" t="s">
-        <v>308</v>
-      </c>
-      <c r="D142" s="19"/>
-      <c r="E142" s="21" t="s">
-        <v>309</v>
-      </c>
-      <c r="F142" s="19"/>
-      <c r="G142" s="19" t="s">
-        <v>310</v>
-      </c>
-      <c r="H142" s="19"/>
-      <c r="I142" s="19"/>
-      <c r="J142" s="19"/>
-      <c r="K142" s="19"/>
-      <c r="L142" s="19"/>
-      <c r="M142" s="19"/>
-      <c r="AMF142" s="19"/>
-      <c r="AMG142" s="19"/>
-      <c r="AMH142" s="19"/>
-      <c r="AMI142" s="19"/>
-      <c r="AMJ142" s="19"/>
-    </row>
-    <row r="143" s="19" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A143" s="20" t="s">
+      <c r="B152" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="C152" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="D152" s="17"/>
+      <c r="E152" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="F152" s="17"/>
+      <c r="G152" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="H152" s="17"/>
+      <c r="I152" s="17"/>
+      <c r="J152" s="17"/>
+      <c r="K152" s="17"/>
+      <c r="L152" s="17"/>
+      <c r="M152" s="17"/>
+      <c r="AMF152" s="17"/>
+      <c r="AMG152" s="17"/>
+      <c r="AMH152" s="17"/>
+      <c r="AMI152" s="17"/>
+      <c r="AMJ152" s="17"/>
+    </row>
+    <row r="153" s="17" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A153" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B143" s="20" t="s">
-        <v>311</v>
-      </c>
-      <c r="C143" s="19" t="s">
-        <v>312</v>
-      </c>
-      <c r="D143" s="19"/>
-      <c r="E143" s="21" t="s">
-        <v>313</v>
-      </c>
-      <c r="F143" s="19"/>
-      <c r="G143" s="19"/>
-      <c r="H143" s="19"/>
-      <c r="I143" s="19"/>
-      <c r="J143" s="19"/>
-      <c r="K143" s="19"/>
-      <c r="L143" s="19"/>
-      <c r="M143" s="19"/>
-      <c r="AMF143" s="19"/>
-      <c r="AMG143" s="19"/>
-      <c r="AMH143" s="19"/>
-      <c r="AMI143" s="19"/>
-      <c r="AMJ143" s="19"/>
-    </row>
-    <row r="144" s="19" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A144" s="20" t="s">
+      <c r="B153" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="C153" s="17" t="s">
+        <v>332</v>
+      </c>
+      <c r="D153" s="17"/>
+      <c r="E153" s="19" t="s">
+        <v>333</v>
+      </c>
+      <c r="F153" s="17"/>
+      <c r="G153" s="17"/>
+      <c r="H153" s="17"/>
+      <c r="I153" s="17"/>
+      <c r="J153" s="17"/>
+      <c r="K153" s="17"/>
+      <c r="L153" s="17"/>
+      <c r="M153" s="17"/>
+      <c r="AMF153" s="17"/>
+      <c r="AMG153" s="17"/>
+      <c r="AMH153" s="17"/>
+      <c r="AMI153" s="17"/>
+      <c r="AMJ153" s="17"/>
+    </row>
+    <row r="154" s="17" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A154" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B144" s="20" t="s">
-        <v>314</v>
-      </c>
-      <c r="C144" s="19" t="s">
+      <c r="B154" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="C154" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="D144" s="19"/>
-      <c r="E144" s="19" t="s">
+      <c r="D154" s="17"/>
+      <c r="E154" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="F144" s="19"/>
-      <c r="G144" s="19" t="s">
+      <c r="F154" s="17"/>
+      <c r="G154" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H144" s="19"/>
-      <c r="I144" s="19"/>
-      <c r="J144" s="19"/>
-      <c r="K144" s="19"/>
-      <c r="L144" s="19"/>
-      <c r="M144" s="19"/>
-      <c r="AMF144" s="19"/>
-      <c r="AMG144" s="19"/>
-      <c r="AMH144" s="19"/>
-      <c r="AMI144" s="19"/>
-      <c r="AMJ144" s="19"/>
-    </row>
-    <row r="145" s="19" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A145" s="20" t="s">
+      <c r="H154" s="17"/>
+      <c r="I154" s="17"/>
+      <c r="J154" s="17"/>
+      <c r="K154" s="17"/>
+      <c r="L154" s="17"/>
+      <c r="M154" s="17"/>
+      <c r="AMF154" s="17"/>
+      <c r="AMG154" s="17"/>
+      <c r="AMH154" s="17"/>
+      <c r="AMI154" s="17"/>
+      <c r="AMJ154" s="17"/>
+    </row>
+    <row r="155" s="17" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A155" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B145" s="20" t="s">
-        <v>315</v>
-      </c>
-      <c r="C145" s="19" t="s">
-        <v>316</v>
-      </c>
-      <c r="D145" s="19"/>
-      <c r="E145" s="19" t="s">
+      <c r="B155" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="C155" s="17" t="s">
+        <v>336</v>
+      </c>
+      <c r="D155" s="17"/>
+      <c r="E155" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="F145" s="19"/>
-      <c r="G145" s="19" t="s">
+      <c r="F155" s="17"/>
+      <c r="G155" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="H145" s="19"/>
-      <c r="I145" s="19"/>
-      <c r="J145" s="19"/>
-      <c r="K145" s="19"/>
-      <c r="L145" s="19"/>
-      <c r="M145" s="19"/>
-      <c r="AMF145" s="19"/>
-      <c r="AMG145" s="19"/>
-      <c r="AMH145" s="19"/>
-      <c r="AMI145" s="19"/>
-      <c r="AMJ145" s="19"/>
-    </row>
-    <row r="146" s="19" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A146" s="20" t="s">
+      <c r="H155" s="17"/>
+      <c r="I155" s="17"/>
+      <c r="J155" s="17"/>
+      <c r="K155" s="17"/>
+      <c r="L155" s="17"/>
+      <c r="M155" s="17"/>
+      <c r="AMF155" s="17"/>
+      <c r="AMG155" s="17"/>
+      <c r="AMH155" s="17"/>
+      <c r="AMI155" s="17"/>
+      <c r="AMJ155" s="17"/>
+    </row>
+    <row r="156" s="17" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A156" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B146" s="20" t="s">
-        <v>317</v>
-      </c>
-      <c r="C146" s="19" t="s">
-        <v>318</v>
-      </c>
-      <c r="D146" s="19"/>
-      <c r="E146" s="21" t="s">
-        <v>309</v>
-      </c>
-      <c r="F146" s="19"/>
-      <c r="G146" s="19"/>
-      <c r="H146" s="19"/>
-      <c r="I146" s="19"/>
-      <c r="J146" s="19"/>
-      <c r="K146" s="19"/>
-      <c r="L146" s="19"/>
-      <c r="M146" s="19"/>
-      <c r="AMF146" s="19"/>
-      <c r="AMG146" s="19"/>
-      <c r="AMH146" s="19"/>
-      <c r="AMI146" s="19"/>
-      <c r="AMJ146" s="19"/>
-    </row>
-    <row r="147" s="19" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A147" s="20" t="s">
+      <c r="B156" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="C156" s="17" t="s">
+        <v>338</v>
+      </c>
+      <c r="D156" s="17"/>
+      <c r="E156" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="F156" s="17"/>
+      <c r="G156" s="17"/>
+      <c r="H156" s="17"/>
+      <c r="I156" s="17"/>
+      <c r="J156" s="17"/>
+      <c r="K156" s="17"/>
+      <c r="L156" s="17"/>
+      <c r="M156" s="17"/>
+      <c r="AMF156" s="17"/>
+      <c r="AMG156" s="17"/>
+      <c r="AMH156" s="17"/>
+      <c r="AMI156" s="17"/>
+      <c r="AMJ156" s="17"/>
+    </row>
+    <row r="157" s="17" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A157" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B147" s="20" t="s">
-        <v>319</v>
-      </c>
-      <c r="C147" s="19" t="s">
-        <v>320</v>
-      </c>
-      <c r="D147" s="19"/>
-      <c r="E147" s="21" t="s">
-        <v>309</v>
-      </c>
-      <c r="F147" s="19"/>
-      <c r="G147" s="19"/>
-      <c r="H147" s="19"/>
-      <c r="I147" s="19"/>
-      <c r="J147" s="19"/>
-      <c r="K147" s="19"/>
-      <c r="L147" s="19"/>
-      <c r="M147" s="19"/>
-      <c r="AMF147" s="19"/>
-      <c r="AMG147" s="19"/>
-      <c r="AMH147" s="19"/>
-      <c r="AMI147" s="19"/>
-      <c r="AMJ147" s="19"/>
-    </row>
-    <row r="148" s="19" customFormat="1" ht="12.75">
-      <c r="A148" s="20" t="s">
+      <c r="B157" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="C157" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="D157" s="17"/>
+      <c r="E157" s="19" t="s">
+        <v>329</v>
+      </c>
+      <c r="F157" s="17"/>
+      <c r="G157" s="17"/>
+      <c r="H157" s="17"/>
+      <c r="I157" s="17"/>
+      <c r="J157" s="17"/>
+      <c r="K157" s="17"/>
+      <c r="L157" s="17"/>
+      <c r="M157" s="17"/>
+      <c r="AMF157" s="17"/>
+      <c r="AMG157" s="17"/>
+      <c r="AMH157" s="17"/>
+      <c r="AMI157" s="17"/>
+      <c r="AMJ157" s="17"/>
+    </row>
+    <row r="158" s="17" customFormat="1" ht="12.75">
+      <c r="A158" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B148" s="20" t="s">
-        <v>321</v>
-      </c>
-      <c r="C148" s="19" t="s">
-        <v>322</v>
-      </c>
-      <c r="D148" s="19"/>
-      <c r="E148" s="19" t="s">
+      <c r="B158" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="C158" s="17" t="s">
+        <v>342</v>
+      </c>
+      <c r="D158" s="17"/>
+      <c r="E158" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="F148" s="19"/>
-      <c r="G148" s="19" t="s">
-        <v>323</v>
-      </c>
-      <c r="H148" s="19"/>
-      <c r="I148" s="19"/>
-      <c r="J148" s="19"/>
-      <c r="K148" s="19"/>
-      <c r="L148" s="19"/>
-      <c r="M148" s="19"/>
-      <c r="AMF148" s="19"/>
-      <c r="AMG148" s="19"/>
-      <c r="AMH148" s="19"/>
-      <c r="AMI148" s="19"/>
-      <c r="AMJ148" s="19"/>
-    </row>
-    <row r="149" s="19" customFormat="1" ht="12.75">
-      <c r="A149" s="20" t="s">
+      <c r="F158" s="17"/>
+      <c r="G158" s="17" t="s">
+        <v>343</v>
+      </c>
+      <c r="H158" s="17"/>
+      <c r="I158" s="17"/>
+      <c r="J158" s="17"/>
+      <c r="K158" s="17"/>
+      <c r="L158" s="17"/>
+      <c r="M158" s="17"/>
+      <c r="AMF158" s="17"/>
+      <c r="AMG158" s="17"/>
+      <c r="AMH158" s="17"/>
+      <c r="AMI158" s="17"/>
+      <c r="AMJ158" s="17"/>
+    </row>
+    <row r="159" s="17" customFormat="1" ht="12.75">
+      <c r="A159" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B149" s="20" t="s">
-        <v>324</v>
-      </c>
-      <c r="C149" s="19" t="s">
-        <v>325</v>
-      </c>
-      <c r="D149" s="19"/>
-      <c r="E149" s="19" t="s">
+      <c r="B159" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="C159" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="D159" s="17"/>
+      <c r="E159" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="F149" s="19"/>
-      <c r="G149" s="19"/>
-      <c r="H149" s="19"/>
-      <c r="I149" s="19"/>
-      <c r="J149" s="19"/>
-      <c r="K149" s="19"/>
-      <c r="L149" s="19"/>
-      <c r="M149" s="19"/>
-      <c r="AMF149" s="19"/>
-      <c r="AMG149" s="19"/>
-      <c r="AMH149" s="19"/>
-      <c r="AMI149" s="19"/>
-      <c r="AMJ149" s="19"/>
-    </row>
-    <row r="150" s="19" customFormat="1" ht="12.75">
-      <c r="A150" s="20" t="s">
+      <c r="F159" s="17"/>
+      <c r="G159" s="17"/>
+      <c r="H159" s="17"/>
+      <c r="I159" s="17"/>
+      <c r="J159" s="17"/>
+      <c r="K159" s="17"/>
+      <c r="L159" s="17"/>
+      <c r="M159" s="17"/>
+      <c r="AMF159" s="17"/>
+      <c r="AMG159" s="17"/>
+      <c r="AMH159" s="17"/>
+      <c r="AMI159" s="17"/>
+      <c r="AMJ159" s="17"/>
+    </row>
+    <row r="160" s="17" customFormat="1" ht="12.75">
+      <c r="A160" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B150" s="20" t="s">
-        <v>326</v>
-      </c>
-      <c r="C150" s="19" t="s">
-        <v>327</v>
-      </c>
-      <c r="D150" s="19"/>
-      <c r="E150" s="19" t="s">
+      <c r="B160" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="C160" s="17" t="s">
+        <v>347</v>
+      </c>
+      <c r="D160" s="17"/>
+      <c r="E160" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="F150" s="19"/>
-      <c r="G150" s="19"/>
-      <c r="H150" s="19"/>
-      <c r="I150" s="19"/>
-      <c r="J150" s="19"/>
-      <c r="K150" s="19"/>
-      <c r="L150" s="19"/>
-      <c r="M150" s="19"/>
-      <c r="AMF150" s="19"/>
-      <c r="AMG150" s="19"/>
-      <c r="AMH150" s="19"/>
-      <c r="AMI150" s="19"/>
-      <c r="AMJ150" s="19"/>
-    </row>
-    <row r="151" s="19" customFormat="1" ht="12.75">
-      <c r="A151" s="20" t="s">
+      <c r="F160" s="17"/>
+      <c r="G160" s="17"/>
+      <c r="H160" s="17"/>
+      <c r="I160" s="17"/>
+      <c r="J160" s="17"/>
+      <c r="K160" s="17"/>
+      <c r="L160" s="17"/>
+      <c r="M160" s="17"/>
+      <c r="AMF160" s="17"/>
+      <c r="AMG160" s="17"/>
+      <c r="AMH160" s="17"/>
+      <c r="AMI160" s="17"/>
+      <c r="AMJ160" s="17"/>
+    </row>
+    <row r="161" s="17" customFormat="1" ht="12.75">
+      <c r="A161" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B151" s="20" t="s">
-        <v>328</v>
-      </c>
-      <c r="C151" s="19" t="s">
-        <v>329</v>
-      </c>
-      <c r="D151" s="19"/>
-      <c r="E151" s="19" t="s">
-        <v>330</v>
-      </c>
-      <c r="F151" s="19"/>
-      <c r="G151" s="19"/>
-      <c r="H151" s="19"/>
-      <c r="I151" s="19"/>
-      <c r="J151" s="19"/>
-      <c r="K151" s="19"/>
-      <c r="L151" s="19"/>
-      <c r="M151" s="19"/>
-      <c r="AMF151" s="19"/>
-      <c r="AMG151" s="19"/>
-      <c r="AMH151" s="19"/>
-      <c r="AMI151" s="19"/>
-      <c r="AMJ151" s="19"/>
-    </row>
-    <row r="152" s="0" customFormat="1" ht="12.75">
-      <c r="E152" s="6"/>
-      <c r="G152" s="6"/>
-    </row>
-    <row r="153" s="19" customFormat="1" ht="12.75">
-      <c r="A153" s="20" t="s">
+      <c r="B161" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="C161" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="D161" s="17"/>
+      <c r="E161" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="F161" s="17"/>
+      <c r="G161" s="17"/>
+      <c r="H161" s="17"/>
+      <c r="I161" s="17"/>
+      <c r="J161" s="17"/>
+      <c r="K161" s="17"/>
+      <c r="L161" s="17"/>
+      <c r="M161" s="17"/>
+      <c r="AMF161" s="17"/>
+      <c r="AMG161" s="17"/>
+      <c r="AMH161" s="17"/>
+      <c r="AMI161" s="17"/>
+      <c r="AMJ161" s="17"/>
+    </row>
+    <row r="162" s="0" customFormat="1" ht="12.75">
+      <c r="E162" s="6"/>
+      <c r="G162" s="6"/>
+    </row>
+    <row r="163" s="17" customFormat="1" ht="12.75">
+      <c r="A163" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B153" s="20" t="s">
-        <v>331</v>
-      </c>
-      <c r="C153" s="19" t="s">
+      <c r="B163" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="C163" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D153" s="19"/>
-      <c r="E153" s="19"/>
-      <c r="F153" s="19"/>
-      <c r="G153" s="19" t="s">
+      <c r="D163" s="17"/>
+      <c r="E163" s="17"/>
+      <c r="F163" s="17"/>
+      <c r="G163" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="H153" s="19"/>
-      <c r="I153" s="19"/>
-      <c r="J153" s="19"/>
-      <c r="K153" s="19"/>
-      <c r="L153" s="19"/>
-      <c r="M153" s="19"/>
-      <c r="AMF153" s="19"/>
-      <c r="AMG153" s="19"/>
-      <c r="AMH153" s="19"/>
-      <c r="AMI153" s="19"/>
-      <c r="AMJ153" s="19"/>
-    </row>
-    <row r="154" s="19" customFormat="1" ht="12.75">
-      <c r="A154" s="20" t="s">
+      <c r="H163" s="17"/>
+      <c r="I163" s="17"/>
+      <c r="J163" s="17"/>
+      <c r="K163" s="17"/>
+      <c r="L163" s="17"/>
+      <c r="M163" s="17"/>
+      <c r="AMF163" s="17"/>
+      <c r="AMG163" s="17"/>
+      <c r="AMH163" s="17"/>
+      <c r="AMI163" s="17"/>
+      <c r="AMJ163" s="17"/>
+    </row>
+    <row r="164" s="17" customFormat="1" ht="12.75">
+      <c r="A164" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B154" s="20" t="s">
-        <v>332</v>
-      </c>
-      <c r="C154" s="19" t="s">
+      <c r="B164" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="C164" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D154" s="19"/>
-      <c r="E154" s="19"/>
-      <c r="F154" s="19" t="s">
-        <v>333</v>
-      </c>
-      <c r="G154" s="19"/>
-      <c r="H154" s="19"/>
-      <c r="I154" s="19"/>
-      <c r="J154" s="19"/>
-      <c r="K154" s="19"/>
-      <c r="L154" s="19"/>
-      <c r="M154" s="19"/>
-      <c r="AMF154" s="19"/>
-      <c r="AMG154" s="19"/>
-      <c r="AMH154" s="19"/>
-      <c r="AMI154" s="19"/>
-      <c r="AMJ154" s="19"/>
-    </row>
-    <row r="155" s="19" customFormat="1" ht="12.75">
-      <c r="A155" s="20" t="s">
+      <c r="D164" s="17"/>
+      <c r="E164" s="17"/>
+      <c r="F164" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="G164" s="17"/>
+      <c r="H164" s="17"/>
+      <c r="I164" s="17"/>
+      <c r="J164" s="17"/>
+      <c r="K164" s="17"/>
+      <c r="L164" s="17"/>
+      <c r="M164" s="17"/>
+      <c r="AMF164" s="17"/>
+      <c r="AMG164" s="17"/>
+      <c r="AMH164" s="17"/>
+      <c r="AMI164" s="17"/>
+      <c r="AMJ164" s="17"/>
+    </row>
+    <row r="165" s="17" customFormat="1" ht="12.75">
+      <c r="A165" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B155" s="20" t="s">
-        <v>334</v>
-      </c>
-      <c r="C155" s="19" t="s">
+      <c r="B165" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C165" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D155" s="19"/>
-      <c r="E155" s="19"/>
-      <c r="F155" s="19" t="s">
-        <v>335</v>
-      </c>
-      <c r="G155" s="19"/>
-      <c r="H155" s="19"/>
-      <c r="I155" s="19"/>
-      <c r="J155" s="19"/>
-      <c r="K155" s="19"/>
-      <c r="L155" s="19"/>
-      <c r="M155" s="19"/>
-      <c r="AMF155" s="19"/>
-      <c r="AMG155" s="19"/>
-      <c r="AMH155" s="19"/>
-      <c r="AMI155" s="19"/>
-      <c r="AMJ155" s="19"/>
-    </row>
-    <row r="156" s="19" customFormat="1" ht="12.75">
-      <c r="A156" s="20" t="s">
+      <c r="D165" s="17"/>
+      <c r="E165" s="17"/>
+      <c r="F165" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="G165" s="17"/>
+      <c r="H165" s="17"/>
+      <c r="I165" s="17"/>
+      <c r="J165" s="17"/>
+      <c r="K165" s="17"/>
+      <c r="L165" s="17"/>
+      <c r="M165" s="17"/>
+      <c r="AMF165" s="17"/>
+      <c r="AMG165" s="17"/>
+      <c r="AMH165" s="17"/>
+      <c r="AMI165" s="17"/>
+      <c r="AMJ165" s="17"/>
+    </row>
+    <row r="166" s="17" customFormat="1" ht="12.75">
+      <c r="A166" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B156" s="20" t="s">
-        <v>331</v>
-      </c>
-      <c r="C156" s="19"/>
-      <c r="D156" s="19"/>
-      <c r="E156" s="19"/>
-      <c r="F156" s="19"/>
-      <c r="G156" s="19"/>
-      <c r="H156" s="19"/>
-      <c r="I156" s="19"/>
-      <c r="J156" s="19"/>
-      <c r="K156" s="19"/>
-      <c r="L156" s="19"/>
-      <c r="M156" s="19"/>
-      <c r="AMF156" s="19"/>
-      <c r="AMG156" s="19"/>
-      <c r="AMH156" s="19"/>
-      <c r="AMI156" s="19"/>
-      <c r="AMJ156" s="19"/>
-    </row>
-    <row r="157" s="0" customFormat="1" ht="12.75">
-      <c r="A157" s="6"/>
-      <c r="B157" s="6"/>
-      <c r="E157" s="6"/>
-      <c r="G157" s="6"/>
-    </row>
-    <row r="158" s="19" customFormat="1" ht="12.75">
-      <c r="A158" s="20" t="s">
+      <c r="B166" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="C166" s="17"/>
+      <c r="D166" s="17"/>
+      <c r="E166" s="17"/>
+      <c r="F166" s="17"/>
+      <c r="G166" s="17"/>
+      <c r="H166" s="17"/>
+      <c r="I166" s="17"/>
+      <c r="J166" s="17"/>
+      <c r="K166" s="17"/>
+      <c r="L166" s="17"/>
+      <c r="M166" s="17"/>
+      <c r="AMF166" s="17"/>
+      <c r="AMG166" s="17"/>
+      <c r="AMH166" s="17"/>
+      <c r="AMI166" s="17"/>
+      <c r="AMJ166" s="17"/>
+    </row>
+    <row r="167" s="0" customFormat="1" ht="12.75">
+      <c r="A167" s="6"/>
+      <c r="B167" s="6"/>
+      <c r="E167" s="6"/>
+      <c r="G167" s="6"/>
+    </row>
+    <row r="168" s="17" customFormat="1" ht="12.75">
+      <c r="A168" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B158" s="20" t="s">
+      <c r="B168" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="C158" s="19"/>
-      <c r="D158" s="19"/>
-      <c r="E158" s="19"/>
-      <c r="F158" s="19"/>
-      <c r="G158" s="19"/>
-      <c r="H158" s="19"/>
-      <c r="I158" s="19"/>
-      <c r="J158" s="19"/>
-      <c r="K158" s="19"/>
-      <c r="L158" s="19"/>
-      <c r="M158" s="19"/>
-      <c r="AMF158" s="19"/>
-      <c r="AMG158" s="19"/>
-      <c r="AMH158" s="19"/>
-      <c r="AMI158" s="19"/>
-      <c r="AMJ158" s="19"/>
-    </row>
-    <row r="159" ht="12.75"/>
-    <row r="160" ht="12.75"/>
-    <row r="161" ht="12.75"/>
-    <row r="162" ht="12.75"/>
-    <row r="163" ht="12.75"/>
-    <row r="164" ht="12.75"/>
-    <row r="165" ht="12.75"/>
-    <row r="166" ht="12.75"/>
-    <row r="167" ht="12.75"/>
-    <row r="168" ht="12.75"/>
+      <c r="C168" s="17"/>
+      <c r="D168" s="17"/>
+      <c r="E168" s="17"/>
+      <c r="F168" s="17"/>
+      <c r="G168" s="17"/>
+      <c r="H168" s="17"/>
+      <c r="I168" s="17"/>
+      <c r="J168" s="17"/>
+      <c r="K168" s="17"/>
+      <c r="L168" s="17"/>
+      <c r="M168" s="17"/>
+      <c r="AMF168" s="17"/>
+      <c r="AMG168" s="17"/>
+      <c r="AMH168" s="17"/>
+      <c r="AMI168" s="17"/>
+      <c r="AMJ168" s="17"/>
+    </row>
+    <row r="169" ht="12.75"/>
     <row r="170" ht="12.75"/>
     <row r="171" ht="12.75"/>
     <row r="172" ht="12.75"/>
@@ -6276,36 +6587,45 @@
     <row r="176" ht="12.75"/>
     <row r="177" ht="12.75"/>
     <row r="178" ht="12.75"/>
-    <row r="179" ht="12.75"/>
     <row r="180" ht="12.75"/>
     <row r="181" ht="12.75"/>
     <row r="182" ht="12.75"/>
+    <row r="183" ht="12.75"/>
+    <row r="184" ht="12.75"/>
+    <row r="185" ht="12.75"/>
     <row r="186" ht="12.75"/>
+    <row r="187" ht="12.75"/>
+    <row r="188" ht="12.75"/>
+    <row r="189" ht="12.75"/>
+    <row r="190" ht="12.75"/>
+    <row r="191" ht="12.75"/>
+    <row r="192" ht="12.75"/>
     <row r="196" ht="12.75"/>
-    <row r="197" ht="12.75"/>
-    <row r="198" ht="12.75"/>
-    <row r="199" ht="12.75"/>
-    <row r="200" ht="12.75"/>
-    <row r="201" ht="12.75"/>
-    <row r="202" ht="12.75"/>
-    <row r="203" ht="12.75"/>
-    <row r="204" ht="12.75"/>
-    <row r="205" ht="12.75"/>
+    <row r="206" ht="12.75"/>
+    <row r="207" ht="12.75"/>
+    <row r="208" ht="12.75"/>
+    <row r="209" ht="12.75"/>
     <row r="210" ht="12.75"/>
     <row r="211" ht="12.75"/>
     <row r="212" ht="12.75"/>
     <row r="213" ht="12.75"/>
     <row r="214" ht="12.75"/>
     <row r="215" ht="12.75"/>
-    <row r="216" ht="12.75"/>
-    <row r="217" ht="12.75"/>
-    <row r="218" ht="12.75"/>
-    <row r="219" ht="12.75"/>
     <row r="220" ht="12.75"/>
     <row r="221" ht="12.75"/>
     <row r="222" ht="12.75"/>
     <row r="223" ht="12.75"/>
     <row r="224" ht="12.75"/>
+    <row r="225" ht="12.75"/>
+    <row r="226" ht="12.75"/>
+    <row r="227" ht="12.75"/>
+    <row r="228" ht="12.75"/>
+    <row r="229" ht="12.75"/>
+    <row r="230" ht="12.75"/>
+    <row r="231" ht="12.75"/>
+    <row r="232" ht="12.75"/>
+    <row r="233" ht="12.75"/>
+    <row r="234" ht="12.75"/>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -6337,7 +6657,7 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
       <c r="A1" s="25" t="s">
-        <v>336</v>
+        <v>356</v>
       </c>
       <c r="B1" s="25" t="s">
         <v>1</v>
@@ -6346,10 +6666,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>337</v>
+        <v>357</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>338</v>
+        <v>358</v>
       </c>
       <c r="F1" s="26"/>
       <c r="G1" s="27"/>
@@ -6375,10 +6695,10 @@
     </row>
     <row r="2" ht="12.75">
       <c r="A2" t="s">
-        <v>339</v>
+        <v>359</v>
       </c>
       <c r="B2" t="s">
-        <v>340</v>
+        <v>360</v>
       </c>
       <c r="C2" t="s">
         <v>217</v>
@@ -6386,10 +6706,10 @@
     </row>
     <row r="3" ht="12.75">
       <c r="A3" t="s">
-        <v>339</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s">
-        <v>341</v>
+        <v>361</v>
       </c>
       <c r="C3" t="s">
         <v>221</v>
@@ -6397,127 +6717,127 @@
     </row>
     <row r="4" ht="12.75">
       <c r="A4" t="s">
-        <v>339</v>
+        <v>359</v>
       </c>
       <c r="B4" t="s">
-        <v>342</v>
+        <v>362</v>
       </c>
       <c r="C4" t="s">
-        <v>343</v>
+        <v>363</v>
       </c>
     </row>
     <row r="5" ht="14.25"/>
     <row r="6" ht="14.25">
       <c r="A6" t="s">
-        <v>344</v>
+        <v>364</v>
       </c>
       <c r="B6" t="s">
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="C6" t="s">
-        <v>346</v>
+        <v>366</v>
       </c>
     </row>
     <row r="7" ht="14.25">
       <c r="A7" t="s">
-        <v>344</v>
+        <v>364</v>
       </c>
       <c r="B7" t="s">
-        <v>347</v>
+        <v>367</v>
       </c>
       <c r="C7" t="s">
-        <v>348</v>
+        <v>368</v>
       </c>
     </row>
     <row r="8" ht="14.25"/>
     <row r="9" ht="14.25">
       <c r="A9" t="s">
-        <v>349</v>
+        <v>369</v>
       </c>
       <c r="B9" t="s">
-        <v>350</v>
+        <v>370</v>
       </c>
       <c r="C9" t="s">
-        <v>351</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10" ht="14.25">
       <c r="A10" t="s">
-        <v>349</v>
+        <v>369</v>
       </c>
       <c r="B10" t="s">
-        <v>352</v>
+        <v>372</v>
       </c>
       <c r="C10" t="s">
-        <v>353</v>
+        <v>373</v>
       </c>
     </row>
     <row r="11" ht="14.25">
       <c r="A11" t="s">
-        <v>349</v>
+        <v>369</v>
       </c>
       <c r="B11" t="s">
-        <v>354</v>
+        <v>374</v>
       </c>
       <c r="C11" t="s">
-        <v>355</v>
+        <v>375</v>
       </c>
     </row>
     <row r="12" ht="14.25"/>
     <row r="13" ht="14.25">
       <c r="A13" t="s">
-        <v>356</v>
+        <v>376</v>
       </c>
       <c r="B13" t="s">
-        <v>357</v>
+        <v>377</v>
       </c>
       <c r="C13" t="s">
-        <v>358</v>
+        <v>378</v>
       </c>
     </row>
     <row r="14" ht="14.25">
       <c r="A14" t="s">
-        <v>356</v>
+        <v>376</v>
       </c>
       <c r="B14" t="s">
-        <v>359</v>
+        <v>379</v>
       </c>
       <c r="C14" t="s">
-        <v>360</v>
+        <v>380</v>
       </c>
     </row>
     <row r="15" ht="14.25"/>
     <row r="16" ht="14.25">
       <c r="A16" t="s">
-        <v>361</v>
+        <v>381</v>
       </c>
       <c r="B16" t="s">
-        <v>362</v>
+        <v>382</v>
       </c>
       <c r="C16" t="s">
-        <v>363</v>
+        <v>383</v>
       </c>
     </row>
     <row r="17" ht="14.25">
       <c r="A17" t="s">
-        <v>361</v>
+        <v>381</v>
       </c>
       <c r="B17" t="s">
-        <v>364</v>
+        <v>384</v>
       </c>
       <c r="C17" t="s">
-        <v>365</v>
+        <v>385</v>
       </c>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" t="s">
-        <v>361</v>
+        <v>381</v>
       </c>
       <c r="B18" t="s">
-        <v>354</v>
+        <v>374</v>
       </c>
       <c r="C18" t="s">
-        <v>355</v>
+        <v>375</v>
       </c>
     </row>
     <row r="19" ht="14.25"/>
@@ -6526,10 +6846,10 @@
         <v>168</v>
       </c>
       <c r="B20" t="s">
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="D20" t="s">
-        <v>366</v>
+        <v>386</v>
       </c>
     </row>
     <row r="21" ht="14.25">
@@ -6537,10 +6857,10 @@
         <v>168</v>
       </c>
       <c r="B21" t="s">
-        <v>347</v>
+        <v>367</v>
       </c>
       <c r="D21" t="s">
-        <v>367</v>
+        <v>387</v>
       </c>
     </row>
     <row r="22" ht="14.25">
@@ -6548,22 +6868,21 @@
     </row>
     <row r="23" ht="14.25">
       <c r="A23" t="s">
-        <v>368</v>
+        <v>388</v>
       </c>
       <c r="B23" t="s">
-        <v>340</v>
+        <v>360</v>
       </c>
       <c r="C23" t="s">
         <v>217</v>
       </c>
-      <c r="D23"/>
     </row>
     <row r="24" ht="14.25">
       <c r="A24" t="s">
-        <v>368</v>
+        <v>388</v>
       </c>
       <c r="B24" t="s">
-        <v>341</v>
+        <v>361</v>
       </c>
       <c r="C24" t="s">
         <v>221</v>
@@ -6571,13 +6890,13 @@
     </row>
     <row r="25" ht="14.25">
       <c r="A25" s="7" t="s">
-        <v>368</v>
+        <v>388</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>342</v>
+        <v>362</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>343</v>
+        <v>363</v>
       </c>
     </row>
     <row r="26" ht="14.25">
@@ -6585,24 +6904,24 @@
     </row>
     <row r="27" ht="14.25">
       <c r="A27" t="s">
-        <v>369</v>
+        <v>389</v>
       </c>
       <c r="B27" t="s">
-        <v>370</v>
+        <v>390</v>
       </c>
       <c r="C27" t="s">
-        <v>371</v>
+        <v>391</v>
       </c>
     </row>
     <row r="28" ht="14.25">
       <c r="A28" t="s">
-        <v>369</v>
+        <v>389</v>
       </c>
       <c r="B28" t="s">
-        <v>372</v>
+        <v>392</v>
       </c>
       <c r="C28" t="s">
-        <v>373</v>
+        <v>393</v>
       </c>
     </row>
     <row r="29" ht="14.25">
@@ -6610,43 +6929,43 @@
     </row>
     <row r="30" ht="14.25">
       <c r="A30" t="s">
-        <v>374</v>
+        <v>394</v>
       </c>
       <c r="B30" t="s">
-        <v>375</v>
+        <v>395</v>
       </c>
       <c r="C30" t="s">
-        <v>376</v>
+        <v>396</v>
       </c>
     </row>
     <row r="31" ht="14.25">
       <c r="A31" t="s">
-        <v>374</v>
+        <v>394</v>
       </c>
       <c r="B31" t="s">
-        <v>377</v>
+        <v>397</v>
       </c>
       <c r="C31" t="s">
-        <v>378</v>
+        <v>398</v>
       </c>
     </row>
     <row r="32" ht="14.25">
       <c r="A32" t="s">
-        <v>374</v>
+        <v>394</v>
       </c>
       <c r="B32" t="s">
-        <v>379</v>
+        <v>399</v>
       </c>
       <c r="C32" t="s">
-        <v>380</v>
+        <v>400</v>
       </c>
     </row>
     <row r="33" ht="14.25">
       <c r="A33" t="s">
-        <v>374</v>
+        <v>394</v>
       </c>
       <c r="B33" t="s">
-        <v>381</v>
+        <v>401</v>
       </c>
       <c r="C33" t="s">
         <v>264</v>
@@ -6657,24 +6976,24 @@
     </row>
     <row r="35" ht="14.25">
       <c r="A35" t="s">
-        <v>382</v>
+        <v>402</v>
       </c>
       <c r="B35" t="s">
-        <v>347</v>
+        <v>367</v>
       </c>
       <c r="C35" t="s">
-        <v>383</v>
+        <v>403</v>
       </c>
     </row>
     <row r="36" ht="14.25">
       <c r="A36" t="s">
-        <v>382</v>
+        <v>402</v>
       </c>
       <c r="B36" t="s">
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="C36" t="s">
-        <v>384</v>
+        <v>404</v>
       </c>
     </row>
     <row r="37" ht="14.25">
@@ -6682,24 +7001,24 @@
     </row>
     <row r="38" ht="14.25">
       <c r="A38" t="s">
-        <v>385</v>
+        <v>405</v>
       </c>
       <c r="B38" t="s">
-        <v>347</v>
+        <v>367</v>
       </c>
       <c r="C38" t="s">
-        <v>383</v>
+        <v>403</v>
       </c>
     </row>
     <row r="39" ht="14.25">
       <c r="A39" t="s">
-        <v>385</v>
+        <v>405</v>
       </c>
       <c r="B39" t="s">
-        <v>345</v>
+        <v>365</v>
       </c>
       <c r="C39" t="s">
-        <v>386</v>
+        <v>406</v>
       </c>
     </row>
     <row r="40" ht="14.25"/>
@@ -6708,10 +7027,10 @@
         <v>186</v>
       </c>
       <c r="B41" t="s">
-        <v>387</v>
+        <v>407</v>
       </c>
       <c r="C41" t="s">
-        <v>388</v>
+        <v>408</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -6722,7 +7041,7 @@
         <v>186</v>
       </c>
       <c r="B42" t="s">
-        <v>389</v>
+        <v>409</v>
       </c>
       <c r="C42" t="s">
         <v>255</v>
@@ -6736,7 +7055,7 @@
         <v>186</v>
       </c>
       <c r="B43" t="s">
-        <v>390</v>
+        <v>410</v>
       </c>
       <c r="C43" t="s">
         <v>258</v>
@@ -6750,7 +7069,7 @@
         <v>186</v>
       </c>
       <c r="B44" t="s">
-        <v>391</v>
+        <v>411</v>
       </c>
       <c r="C44" t="s">
         <v>261</v>
@@ -6764,10 +7083,10 @@
         <v>186</v>
       </c>
       <c r="B45" t="s">
-        <v>381</v>
+        <v>401</v>
       </c>
       <c r="C45" t="s">
-        <v>392</v>
+        <v>412</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -9710,43 +10029,43 @@
   <sheetData>
     <row r="1" ht="12.800000000000001">
       <c r="A1" s="28" t="s">
-        <v>393</v>
+        <v>413</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>394</v>
+        <v>414</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>395</v>
+        <v>415</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>396</v>
+        <v>416</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>397</v>
+        <v>417</v>
       </c>
       <c r="F1" s="28" t="s">
-        <v>398</v>
+        <v>418</v>
       </c>
     </row>
     <row r="2" ht="12.800000000000001">
       <c r="A2" s="29" t="s">
-        <v>399</v>
+        <v>419</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>400</v>
+        <v>420</v>
       </c>
       <c r="C2" s="30">
         <f ca="1">TODAY()</f>
         <v>44901</v>
       </c>
       <c r="D2" t="s">
-        <v>401</v>
+        <v>421</v>
       </c>
       <c r="E2" t="s">
-        <v>402</v>
+        <v>422</v>
       </c>
       <c r="F2" t="s">
-        <v>403</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>

</xml_diff>